<commit_message>
corrected a silly error
</commit_message>
<xml_diff>
--- a/100_multichoice.xlsx
+++ b/100_multichoice.xlsx
@@ -531,7 +531,11 @@
           <t>name</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr"/>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>questiontext</t>
+        </is>
+      </c>
       <c r="I1" s="4" t="inlineStr">
         <is>
           <t>questiontextformat</t>
@@ -633,7 +637,11 @@
           <t>The type of tooth with pointed edges and one root is mainly used for .</t>
         </is>
       </c>
-      <c r="H2" s="3" t="inlineStr"/>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>The type of tooth with pointed edges and one root is mainly used for ____________.</t>
+        </is>
+      </c>
       <c r="I2" s="3" t="n">
         <v>1</v>
       </c>
@@ -710,7 +718,11 @@
           <t>We should always brush our teeth .</t>
         </is>
       </c>
-      <c r="H3" s="3" t="inlineStr"/>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>We should always brush our teeth  _______ .</t>
+        </is>
+      </c>
       <c r="I3" s="3" t="n">
         <v>1</v>
       </c>
@@ -787,7 +799,11 @@
           <t>The diagram below represents a tooth.</t>
         </is>
       </c>
-      <c r="H4" s="3" t="inlineStr"/>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>The diagram below represents a tooth.Which of the following statements is trueabout the tooth above?</t>
+        </is>
+      </c>
       <c r="I4" s="3" t="n">
         <v>1</v>
       </c>
@@ -864,7 +880,11 @@
           <t>The first phase of the moon observed after the new moon is known as .</t>
         </is>
       </c>
-      <c r="H5" s="3" t="inlineStr"/>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>The first phase of the moon observed afterthe new moon is known as .</t>
+        </is>
+      </c>
       <c r="I5" s="3" t="n">
         <v>1</v>
       </c>
@@ -941,7 +961,11 @@
           <t>Which one of the following can not be seen in the sky at night?</t>
         </is>
       </c>
-      <c r="H6" s="3" t="inlineStr"/>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following can not be seen inthe sky at night?</t>
+        </is>
+      </c>
       <c r="I6" s="3" t="n">
         <v>1</v>
       </c>
@@ -1018,7 +1042,11 @@
           <t>A lump of soil was put into a container full of water as shown below.</t>
         </is>
       </c>
-      <c r="H7" s="3" t="inlineStr"/>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>A lump of soil was put into a container full ofwater as shown below.Which of the following components of soilwas being investigated?</t>
+        </is>
+      </c>
       <c r="I7" s="3" t="n">
         <v>1</v>
       </c>
@@ -1095,7 +1123,11 @@
           <t>Which one of the following is not a cutting tool?</t>
         </is>
       </c>
-      <c r="H8" s="3" t="inlineStr"/>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not a cutting tool?</t>
+        </is>
+      </c>
       <c r="I8" s="3" t="n">
         <v>1</v>
       </c>
@@ -1172,7 +1204,11 @@
           <t>Which one of the following animals do not live in soil?</t>
         </is>
       </c>
-      <c r="H9" s="3" t="inlineStr"/>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following animals do notlive in soil?</t>
+        </is>
+      </c>
       <c r="I9" s="3" t="n">
         <v>1</v>
       </c>
@@ -1249,7 +1285,11 @@
           <t>Which one of the following is not a protective food?</t>
         </is>
       </c>
-      <c r="H10" s="3" t="inlineStr"/>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not a protectivefood?</t>
+        </is>
+      </c>
       <c r="I10" s="3" t="n">
         <v>1</v>
       </c>
@@ -1326,7 +1366,11 @@
           <t>We eat a balanced diet in order to</t>
         </is>
       </c>
-      <c r="H11" s="3" t="inlineStr"/>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>We eat a balanced diet in order to</t>
+        </is>
+      </c>
       <c r="I11" s="3" t="n">
         <v>1</v>
       </c>
@@ -1403,7 +1447,11 @@
           <t>Which one of the following animals can not move by flying?</t>
         </is>
       </c>
-      <c r="H12" s="3" t="inlineStr"/>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following animals can notmove by flying?</t>
+        </is>
+      </c>
       <c r="I12" s="3" t="n">
         <v>1</v>
       </c>
@@ -1480,7 +1528,11 @@
           <t>When a bottle top is rolled into a ball, it sinks. Which of the following factors mainly makes this happen?</t>
         </is>
       </c>
-      <c r="H13" s="3" t="inlineStr"/>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>When a bottle top is rolled into a ball, it sinks.Which of the following factors mainly makesthis happen?</t>
+        </is>
+      </c>
       <c r="I13" s="3" t="n">
         <v>1</v>
       </c>
@@ -1557,7 +1609,11 @@
           <t>The following The following are oil crops exceptare oil crops except</t>
         </is>
       </c>
-      <c r="H14" s="3" t="inlineStr"/>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>The following are oil crops except</t>
+        </is>
+      </c>
       <c r="I14" s="3" t="n">
         <v>1</v>
       </c>
@@ -1634,7 +1690,11 @@
           <t>Which one of the following is the correct meaning of letter D in AIDS?</t>
         </is>
       </c>
-      <c r="H15" s="3" t="inlineStr"/>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is the correctmeaning of letter D in AIDS?</t>
+        </is>
+      </c>
       <c r="I15" s="3" t="n">
         <v>1</v>
       </c>
@@ -1711,7 +1771,11 @@
           <t>Which one of the followiWhich one of the following personal item should not be shared?ng personal things should not be shared?</t>
         </is>
       </c>
-      <c r="H16" s="3" t="inlineStr"/>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following personal item should not be shared?</t>
+        </is>
+      </c>
       <c r="I16" s="3" t="n">
         <v>1</v>
       </c>
@@ -1788,7 +1852,11 @@
           <t>Which one of the following is used by many homes in Kenya to store water?</t>
         </is>
       </c>
-      <c r="H17" s="3" t="inlineStr"/>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is used by manyhomes in Kenya to store water?</t>
+        </is>
+      </c>
       <c r="I17" s="3" t="n">
         <v>1</v>
       </c>
@@ -1865,7 +1933,22 @@
           <t>A pupil matched different materials in a table as shown below.</t>
         </is>
       </c>
-      <c r="H18" s="6" t="inlineStr"/>
+      <c r="H18" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A pupil matched different materials in a table as shown below. Which two materials were wrongly grouped?
+Floats
+Sinks
+Rubber band
+Iron nail
+Wood
+Candle wax
+Glass
+Stainless Steel spoon
+Feather
+Plasticine
+</t>
+        </is>
+      </c>
       <c r="I18" s="3" t="n">
         <v>1</v>
       </c>
@@ -1942,7 +2025,11 @@
           <t>Goats in Kenya are mainly kept for .</t>
         </is>
       </c>
-      <c r="H19" s="3" t="inlineStr"/>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>Goats in Kenya are mainly kept for .</t>
+        </is>
+      </c>
       <c r="I19" s="3" t="n">
         <v>1</v>
       </c>
@@ -2019,7 +2106,11 @@
           <t>Weeds caWeeds can best be removed from a kitchen garden by .n best be removed from a kitchen garden by .</t>
         </is>
       </c>
-      <c r="H20" s="3" t="inlineStr"/>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>Weeds can best be removed from a kitchengarden by .</t>
+        </is>
+      </c>
       <c r="I20" s="3" t="n">
         <v>1</v>
       </c>
@@ -2096,7 +2187,11 @@
           <t>Which one of the following weeds is known for its strong bad smell?</t>
         </is>
       </c>
-      <c r="H21" s="3" t="inlineStr"/>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following weeds is knownfor its strong bad smell?</t>
+        </is>
+      </c>
       <c r="I21" s="3" t="n">
         <v>1</v>
       </c>
@@ -2173,7 +2268,11 @@
           <t>Which one of the following practices can help in maintaining good healthy teeth?</t>
         </is>
       </c>
-      <c r="H22" s="3" t="inlineStr"/>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following practices can helpin maintaining good healthy teeth?</t>
+        </is>
+      </c>
       <c r="I22" s="3" t="n">
         <v>1</v>
       </c>
@@ -2250,7 +2349,11 @@
           <t>Which one of the following cannot be made from fibre?</t>
         </is>
       </c>
-      <c r="H23" s="3" t="inlineStr"/>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following cannot be madefrom fibre?</t>
+        </is>
+      </c>
       <c r="I23" s="3" t="n">
         <v>1</v>
       </c>
@@ -2327,7 +2430,11 @@
           <t>Mary weighs 25 kg and Tom weighs 35 kg. They sat on a see saw as shown in the diagram below.</t>
         </is>
       </c>
-      <c r="H24" s="3" t="inlineStr"/>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>Mary weighs 25 kg and Tom weighs 35 kg. They sat on a see saw as shown in thediagram below.&lt;img src="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAXgAAADKCAIAAAAgisw7AAAgAElEQVR4nOx991sVx/e//0lMUN9qLI8N847GmJhijUZjAHtHFAGRIgKCoAKKIAgqgoKKir2jsRdQsUtHFAQVlF5uv7uz3x/O+54Ms3v37m1Kvp+ch4dn7+6UM+W85syZMzM9hH/pX/qX/iUnU4/PzcC/9C/9S///Uw+O43ieJxTBT0EQeJ4XBAGegTAMvqff4E8mD0iH53k6QUIIx3HwIJmR88psD9GMAdvmgiksgjhYty27o0h5AZVXo5JcmDe2pSwZS8ynOYmgxYcRN4WZWsu2fD3gsxI27KEeRqMRS04jDjLBoAPihUBVFlN9kgUT4xH9UxCVv3vKm8Imt4d5q+LaX1H2d1wbcrQKXh3VExRihEx0JX3bXKaSksJxnLm4jHRYy5tCaaKBxmIu9lAPLDZdZoQYpnYESgERutadGHSYYtAvOY4TV7F8dTuVlOci0/xOlQcZNuzM19oexjSxnWRVYa2NKBlFLJDK05dsdJkKYWSBiPQXFDGZvJSUlE5HzI85QaOZp7uBM4TubxsNzSWiAOmqwggUJAmilpMppzgRyWAOL57DyarmtzOLbktWcWh/cT4lqNmQjgzsEikSCwL+nDBhkssXPS/mXhEn2Nra5jrc1eWLnvK8KRk2MHFxYBnQtJNYYzCdE/w3GIwMWKI+IlkAc/DMGGJIV80IHpiSd2eRcwZvMhXYrchaDu0sUbcCGloOLbYXAzHi6JJA4zrctbq6hknH3X2Wyxc95YHG4ijI5IgsgaFWSYlsph4MfzTowjMYcRikIFJGLMbEIy4k/cBMpsRgT3+yv5wW28CqRBS+V5imkujdB30kBxirmsnaNpU3ult8o/ArdkvmJZB4ZMUlDpQIrVarUqm0Wh0xQ4LIHMH0eQAaly96urvPam1tw/cbojbCezHQ0JJorjbwv7ilkAcsJsdxRqNRpg5tox4C1fCoqjCYQlcTLhWJWafrjim5uGxECmWs7TfKyVHpODZxccM7KmXludsTHZ+tXbOwKrBDVvcsEpMO3T/F6EBnDQEu/3Vt2bLl8+cvDF677u3b94SCFTpN8XoLHQCAJj0jy+WLnhuiNsJL/AlfJWtAsiOJBVn8H2wa+IBkf30y9DfQEBOeYV1gfpi3pKkFeSVS8yNxqxAz5mTJl44qp50SJdkL6WLaw5K56DI14CTpkv/K8CPWSR3CkkU26BwtZqqcK+yBYnSAn1VVb5qamlUqlUajISYdB6J0dHR++823/f/Td+jgIQP7D5g1a45arWY6idC1lsRAQwhBKAEVJj0jKy//ASg4LS2tDNBUV9d4enqBmgMPEyZMgk/wXF1d4+4+y3W4K2AWIQTDQL7wExgwGo2gyDgLaOgGQ2yj6x2fJduViPCe/sT8xJcyC+ROIscCjUNytJMlm+PanI6z28haciwzhBB6yoASodXqkpJ3rljhPWfOPA+P2UuXevr4+F26fLWtrR1DlpVV9P7KpY9Lr6/79uv9lUvfXr3TM7IUVhctFwglra1tYJRxHe7qOtz1RWGxYNJ3IBbYhgFEEhKTITADNJ6eXqAHIbjQYTAYsoGy6VygoXMiXac/NDowdSdTm/iJQXGBqlz5FOikZNJ3NnUr6fqXnEQcx71/XwfP0OJNTc2J21OGDh7S+yuXEcNGeHjMHjRg4Ny5889fuPTzz7/+8sv4m7fu6vWG0tLytSGhvb9ygb8+Lr36uPQaPHAQoAMjAuYIAtBQUl1dA8tMOUdPwhv6a0BgsMsXPXMvXcHoDNC4DndNz8gSBOFFYTE8kK4qDP2TUNqckzz3umg0DKYIUq40NBOkq2GFCWMOCMwlaBGwxO+dhL7ijP6hiTuWnMSqucY1F5jpq0z3sIdJrVaL0Q0G4/qIDb16fol/fXv17v2VS6+eX37dt1/fXr379e7T+yuXM2cvhoSETpkyFSAGA/f+ymVbQpI5Zd8cMZOjnKMnExKTJb9OmDDJ3X0WvWhDgwiNILR8Me/pn7SbvrOARmxhISbbsAyOCFImG/GDJOgw5beZe6wgO9P5BCQjORbDKEzKgdQ9K9MqoVUYjA6PDwaD8eSpcwP69UdAGTZk6O60vfAMgAL6y6j/jlq61LOionL27LkAQ/g1ZF2YtTxImnslvwJG0F6v4qmTuFzMe8Zkw4i/Y6kHjQWMc7DRaKTzZlBDElYEEbhY5N7OUkl69DiQHJu4uB5sTt95pVYoxraFcVTxLWZtlcAwgTP27v9m5Dfjx08cMmhw///07f2Vi/cq329GfgPayrfffDtsyFBAkz4uvaZP/0OvNxSXlA0aMJDWaLL2H4KRGAZsJbMSgBJzYcQaDV1MSaBhZNAc0AA5dczugYnSFQHMgQzTXsJIMoqM5E+nSoW1iVsV3mJga1OzKGnmSuSkocYqspMBum9Y7Bg2VIL97IEIhIVHbI7Z4uExu1/vPkMGDQb7LuoyOEVy+aJnH5defXv1Liwq4Xnew2M2vIGvV6/dZOYEFvlXDjRgo7mYewXTFAMNMc1LkACeIEx1dQ0zk2Ik17H0t42GXgkSTPMmgVIZ8L84sCR9GqBxNnUfzj8jJ47tgkRkCLAKQ51UDzT2+fj4lZVVbI7ZMmvWnLPncgcNGDigX3+YGcF/QBkEnbDwCK1Wt2lzHBqD+/bqXVb+0lpWlU+dcEdCQGBwQmIyuhSDeZgx+gomX6RtCUkuX/RMSEzOOXoSF6o+AcoI6EcjXmPC/MRmGqtM03SyzijAJyNGMD4jA584dwe2HXZ6e0z4SjQdexhub++YOdOto6PTaDS2tLQKgnD12s1ff50A4AKmGfTTBSPxiGEjamvfnTp93uWLnn179e7j0mv8+IkdHZ3WZq0caARBaG1tA70G4CY9I2vChEmFRSUCBTQ4HQGBbW5u2RC10XW4q7v7rCM5J8QaDek6WXEgsUCDnNHbHxitRLKjMPAk+VWGD3MBuic8dU+u7CSZtvvEOZoL8Gm0nvx7DyIio3ieNxqNBoNRp9PX138MCQld5ukVGrYerTAINP3/09d1uOut23lLl3qm7dmXkpqWkLhjmafXp1kPlRc6ZtmLMY8AQtEC7jyFoIsfjWAyCAHQ4FE1gmnzAQN+4gLbvDYmj1COKrwSvHNIRjbTZ2Tgk2WtvAlsABp7VmchYvKOXadOn4MOD6TT6Wtr37W0tC5evJSePeHa04hhI4KCQ/Ly7/M8/6KweF1oeGFRCTM8fwISVxftZ0sIeVFYjD9hZ8Oe9Ew6vPOwpgcNEKiqiPGP3p0giORfBoAEBeItQzbElQnP8GwxrkynF6zc7CcTTFx7SgTss2OineTYlkWy0w2EEBISEnr7Tn5TUzOMrHq9Qa83EEKevyga2H/AwP4DaH8Z+Ptm5DcNDU0gMlqtrr294xO3jljQaLmGN+AB6O4+KyExGSZQEyZMgrkh0wNx+cmB9L9VJ2aXB8INWoLp3QmClb38s1S6/Ceb1VqmIW1LRHkudoZxCP0jEM1RzUEICQ1b//p1tb9/QEBg8JOnz3me1+sNOp2+ra190aIlU6ZMHTv2h19+Ge863BVQpl/vPt+NHtPc3GJ/7sqZlHwjOYjSMrsnPRM3iHt6eoFBR+hqDHHiFgRBhIgILvQcT6AASDzkymDQp+yp8h0OS2cVZku2n8VCSTY2zSRdsTJxZdL/NBX7efFUeVKSyqDyXIhJc1+5ctXLl6/q6z/4+vkP6Nf/SM4JrVar1Wp5ng8NWz9v3oJff52wI2X3ggWLXL7o+XXffmPH/jB58m8ajcZRZbHIJyOz4v/mvE/oPkMrO+Axh+qMU4BG0iWPZpc+dlMJ0HQTMifA5rqj8xiQrC6Z8HZmZz8p4da2pMRfrcUFi6OIzYTRo6I3JSTuOH/h0uaYLbvT9gYEBr98+Uqr1b19+97DY3Ze/v0LF//6/fcZgwcOAnXm6779NkRt/GSjKTPsif8LZvoezaHRaKTdVhBoBKedUt5lC4J4jCVd9xPJL2ybK9Vnoc/LAI1oVo2odmbXPUlJhxH/tDYp5YFlEieENDQ0/frrhOC164YMGhwUHPLhQwPYaN6+fX/8xJnJk3+bO3f+9Ol/gBkY7MG3bud9rvpnFAXmq+SYwWwAIHas4SinHsSMoiVQUwx8SU+mxGl1K6ARu4QJdnBlVUSmimzI2gYJEbqB2cjawJKCYYNG45CCYwocx02cOPnNm9pFi5a4fNHz2fNCPD5Cq9WWlVX8+uuE78eM/W70GNzcVFn52hxv9lB1dU1AYDA45oFJhW5o9OWBv4TEZElYob2NEZWwi+IbcT04ltjlbcyMfkn/lAEamj470DCFcmBHtEiSs0iHV8hnr2FnkJJ+5dSCE0L2ZR5c7R8AFpmExGSdTo8TDUJIc3PLH3/8OWHCJJg6wezp8JHjzhhiAWLgQBlw/IVFIsgFPm1LSEpITE5ITIbtCOLiINCIZZxeZabfO4p/mnpg6mLJZHyCha7LUs6oWceSZKe0mVtzY6nFwFZFVBKSHp2sTc0ZZE/ukoOwMzJSyMntO/k//DCupuYtHpUNR8+BW41eb8i/9+Bi7pWxY38IC4/o49JrbUhoWHiE9ypfMAY7lkN391m4MIRn7iG39M5JyeggpBaBhpFlZ9lomAzoKR9zrCeRWloi3c8M7FSSH1FpHZB+KQ6mvNLksVKcncUotpFVyKhc72B6lJK6lYzuKPrryvVFi5bQoyltKFWpVCOGjXAd7hoVvenmrbsD+w/4um+/Y8dPj3QdmZScajAYzfFpG9F3IYj3QCLQgH2DAQj0sGWARowpDNA4kH+aujjsCV1n+2KxkXz4vMPpJyaLQ64SIbcTaOSzs8jkpyf5ItAPFkMyRbbYHFbxyfN8ff2HSZOmBAYGHzh4BEwzADQwe+I47vCR47Fx8cUlZbDwlJCYvP/A4VH/HTVowMCo6E2vXlVZlaNVJHnir2BGw0UHDtwhBcFgexSc2kcIqap6Iz542ClAg5wx+yAwM3rViXQlh3PjEHISbzanKcYUyQo0l74SKbU5gJ2kMH0lfCoBGmZAdmzxcd2juLh03I8/jfnu+6amZkEQAGXAbQ8PTlm2bLmbm8f8+QufPHn2yy/jS0vL//zT/eu+/X75ZfztO/nOqHY4pRwO3KOBBrZiC111Q0JNTWigYeZfLS2tcPBw5IbobQlJuJ/bKX40yJwYUAQTNHYfc8BnJOW6gwyC2IbUNtd5dx4PJMmqOnF40SBBo9E4b96CO3fzjUZjdXVNS0sr7K4khGi1Oo1Gs2lzXERk1JGcE4sWLZk69fe/rlw3Go237+RPn/6H3+o18+Yt2H/gsMO9+EETgXOIBROCTJgwCQzG7u6zmpqaxeoez/MINHvSM+lbXAghawKC8GJMGrycCDQ4o0MmEGjExiEicr1xOFv2k0J9QRxGyehqQ7JMFjIp0GHwEgz5jLphE1hk2KoS0Y1C91KFqVlFer0hIDDY29tn4cLFP//86+kzF6AVdDq9Xm9ISk719w84dz531qw5o/47asmSZU1NzbmXrri5eexI2f3+fV1jY3NYeETqzj3iUthMoM4wO60FU8Fhe+SagCAMT1cIAE3upSt4bQtKNH1Mn0AZmJ3Rnf4GGnrdmnRdaTc3bnfD/o1kjxZgMQVJdFBeSwzQmIsoCAJeG2gz0JhL3yGjlmRdiYcfyRpQ6Pkpn4jMVyWfzJFeb7h1O8/NzePsuVxBEOCwCLVaXV5R+e033+7clT6w/4Ct8dsvXb46efJvCxYs6te7z42bt41Go1arg11Rkyf/9uFDg+CgeobrmVpaWhlsxfkRBJC0tALQwH+cZMEn1F+YN04EGvreW3xAwtDdGVmsIsbZifnDWyyUkzxeSL60GF6hIDG5MyFlxgmZBBWSk/qDwjHMebkLgsDzfFJy6slT51pb27RanV5vePny1ZQpUwcNGPjd6DGHjxxXqVR6vaG29p2Pj9/B7ByO49RqtVarNRiMRqPx5KlzsXHxDkEZMKzkHD1J6wFMi4N5hZjugKRDAsRUV9fAPAu8/kCu8SoFjOVEoAGe9HoDrnXRzjIM0DDuPeKx659C4OMEf9AS9BvminUZUo4FdDAx0Ei+NJeR+KU5oLGoOChh2B6SVEOUaB8Wu5b4qwN7IyRy6vT5IYMGL13qqdcb6us//P77jPHjJw4dPCQoOITneZVKBbYbMN/AspRWqzMYjFqtTqvVzpo1By+Ksplyjp5EwwoWkOO4PemZWFiYOnl6ehHqqG+sB7TRFBaVgOn3+YsiSARtNHj4lHOBRjBtf2BUL3NAA2RuCP3Hkfj8RItibwOZqy75n/LvP+Owby3R9elALJBMX2EUi+k3NTVnZmUvWbIsIjJ65kw3L6+VidtTRv131MyZbkePnWpoaDIYjDzPGwxGWJDiTWetAPpcvXYzKGitPUoNQAM6B8NfekYWx3HgKAwqCajhefn3JQcwunu/KCwGrGltbeN5vrm5Bb4GBAbHb9uOkyxnGYPRMY/21iNSFl8mABbG4Wx9SpI/qNVaomvD3MK2uShKBuTPqJ7YRvaAixLdB38qqTpr2eB5vrW1LTMr+8mTZ+3tHX/+6X7ufO6LwuKw8IgpU6ampKZptVoQH1QKQHAMBiPHcQmJO+7dL5AviDnCW3HFe5qMRiNzssyLwmJmMQf/03udCCFwVLC7+6zq6hpCSGtrG+g1ADcuX/QcP36iUw6+wrkSzNPwAzOToidNREQOZ8tmklRGJPlkdEv6K86nJkyYFBAY3Nrahl/hJRwEDW3T2tqWc/Qk/gSLHW86YYPJUeypRAihj0yVgSFzAQSqXSQnSrYNCZI1qTAiw5VV0SV5UPJeIUYrR3P4j61TX//Rzc1Do9FotTpCyIvC4gULFqWkpkEra7VaCEkLVH39x32ZBxWyZ5GQc+bIcfhKdzna7GKu1yHRjsUuX/Rctmy5U4BGrzcIpj5KLzxhZdE/mTJ3K4gBkuma5qIwGg3Y3uDEQ8B4d/dZra1t8BWwn/nqOtw1ITEZRgbYRMvUD9Yh3YQQgD4ZRJJP5UBjrvh2tpSdrWxtcyhJyjagkYmrJMr+A4ez9h+CpaWmpma93vDuXd38+QsrX1WBOkOftw1qjl5viNwQjZu/7a9JGgFJ1xsf0fohiACFnprQ0ZubW3C1m+d5cLTZnbbXiUAjiDwLseIEqbahOe4OZJEThUAD7ga0UxNY2vANIAumhiZ9YlJTmSkunS+tMxKTIsMEVlKldB8S52JPVdhA1mbH9ByrojNyYj2z/0uEGQaUMEAIWRMQdOPmHUKIwWDcsjXB29unrq6+rq7+YHYODNK0RqPXG0CCjh0/LblgZBX/5oCV0QzonxgLzayEMhVDyDUBQa7DXTdEbcRR03W4a2Njs1NsNLTOIlAVATUlmCra3J17nxhrrO2X2LrMehn9LL4AEFad6AC4qcSl69VcEBf33cnblenc4RharHlzY4gMgpjrDZJyaC4dhisl1WsOI5T3BEmZodOniyAGYkac5EkGxxWKE0aJ27LtydPnAB9Go3FrfGJo2HpC6S9I+JLjuA8fGlauXIXzL3pV12aCguAeTtSkGM2FKTsiIDL8orA4IDAYz6DwXxP4+nU16l+Opb+BBgEFuaehh1kz67ZkTopkOGeuNKaRgpj0FHgJ1n4x0GCLStqVabBDNlC7kcRrJWybE1dJXDMXUR4s5JubYdKBfUMMN+J87c/O2hRCw9aXlVWAl7DBYNRoNFHRmz5+bNTp9HRT0ksrEHjlylVwEwsDBPZwjmAhUNXFENf1Lm1EQPp4HRq14RwMZ50ZTLraihCb6TMi/rlAY+4TTWKNBq6/ESigwf34Ll3vRWeQhf5JN7lAAQ3Tiub0RIVCzkQUZCHGIinHHTGfkjUvw4lMb5avATHQmAMj+VhWEcdxXl4r37yppQVEo9HwPK/T6eGBNy1vg4SD5x4h5N79An//AKau7BElQvnTMu/F/Q2FF//zlK8Ngg7O/oBzm3kzR+yZwfjMd/X8+UegDJC1DMvYaASTNxTumrUKaOjhgn6gc5cEGnPlYgSYiEicvgxZDCkPNGLO5VNgimYRHcRlpNOxmDWTlLWVw5Beb/D3D2htbQPswDUdjuNgdwK4vArUtkEcrXU6/Sofv9NnLsgU1iqi4YNpevFPZINWtVAhAlcgwTSVgdI5BWhoBUygmgSB2eZ+/LlIhk/xCCBYv+oknjphXLFGI3S1sotZwtm7fMVKzu0ZlKE1U7E0inmQfLa5fS1GNDdxsMiSbdkJsj1BsnJkCDSajo5OlFikt2/fg1IDvjPYUqj4GAzG+voPixYtwV5kJzEtTigTpGQfIF3NwHjCDl0WxE3GzcVR1IPpvsxMEkXFXMftDiTTk8wxTMuV+KxD9KNxHe4KnjIYkTnlzBzQiKtRXpyIpaumsO/KiCIzaRe3rGQNMGyYY0AGHfCNTG3T8iD5yWJLWUsWU7aKOI7zWuHd3t4BZhdiMmp0dHRu2hyr0+lhooRyS58ECo7CKalp+fceCNZjHFMofECko+UU9QNeZBiGB1jkIV0nTbQ9Gw8McCz1YCZ7WIOEwsVuDjSSpJBhJpiMGJuLaC4ji6LL5GIxO/l0BNFBzkqmNvhJOZ/mIsonQvsKWUUWwUtJM9mQL0OtrW3z5y+E+RGNI+UVlaFh6zmOg/1NxDRgMEYQg8FYVv4yKGgtuq05qjaYoYUzOSibG+c40fm8hLLMgpojHg/sp7+BhgZIxihNzwYdzoGTSGEXtKdQ8tElgUZS8hVCkmT69DMvMgnZBjTyss38lI+LAWC3ocUWkYwrwwwdQBzSgT32+YuitD37UBxQJi9dvpqekaXXGzQaTVtbOz2FQSUUlqWMRqOv7+pjx0/b2eUY3dYc0NDFR/jA98xUC5ei8MRSh1QaTX9ft4JZCl1riojGxn8EWWTY/hJZJTbil1YBjcXeyQieOE15oJFMSiauktoj1FzJYt9VAhMymGLVS6sI2Mg5ejIv/wE6TOEkZdPm2Bs372g0GjgWC78KlFKDAvz4ybPvRo85cPAIulDZxgzzIHQ9bxe1LWQAGaPxCJ8RnhBAnQg0NBBiMZB1vqvnj8OZcAYp59NcbxYHo1tX3uRhLh0Z6ZWRIknUsFhAejosZtgqVuVfmkvTHORJBrOTGHB0VLJIEZHRJaXlvGlnNginSqWaMmXq69fVcMQnvqfFGH7COTWEkHv3C5Yu9Vy4cLFarbatmPQzEm2e46h95IJproRWGNL1zBpAFjRjG03koGr7m3oIpo3tCIGSZqR/Cr7YQOKiSdqkxD+ZKJLJMhIurkkGv8TpS2IENo24OJKmGSJy3zJXIiX4ItMZxHBprvNIVq+42q3NV+bZBkKhWLrUs6OjU6AuRdDrDYVFJe7us3Q6vU6n57uuH9NaA3iB8zwPDw0NTWO++76oqESQrXN5rug+Qzvg0YBCh4epKz1HQbsMmrFppcaeSpOkvzUaxnrEjIf/p4BGHMBiDSisHzodGXlQKNgyAiwpw/KBFYqx/WSbdIlTMPfS4X21paXV18+fnlmAoCYkJu9JzwQbMG0HoRe5BUEAMw0cW6PXG9Rq9fUbt6dP/wNWM23mFqtRUngJZYgRRDZg1HFouwwNlA6rOxP9fUwEckDrXYIz268bkkIJtxhRJoBFwFIi+fIpiAc0BmvkBVVh1kqASQxw9vci+XydMS4+ffYC9xDAEhLHcW1t7W5uHh8+NKjVatJVi6FXiwWT0gHbvrVaXXNzi15v2LQ57tbtPBv4ZBqRBhd6qYuuB1rGERARaxiHGmcBDRqZeZObIIOO/3eAhpZw8YOdySpMgR6RxJ8svlEeUjk/Fj8xXYX+SRspbcjCqvBM7lalKUM8zx84eKStrR2HfQCa8xcuhYVH8DwPGg0aaARBwDActWMZTjhva2tvaGjSanWxcfGZWdkOgV0aaHhqTYqjPPQQgxgjCd4kQ8MNnujgQOpBKCM5jceEMtY4PNduSJ6eXnhsYnpGFl1qPMrM4unlzAYFmuwU7E/TEDJ4JM+A5CeFMm9tuRyOXBZTS0reCYYMJK1Wu3Sp55atCWDoRb0ANyjAT5BhlHCdTt/ZqVKpVOkZWWPH/lBWVmEPwzSw0koKpkbLNcoyrbngBlEGaHQ6vYMq72/qgbyisZrWuxw+PthDDCeM5kUHk3yWITicFTZPApTgbX6CCWiY08uxmemMZIBGSYkkAygsi/w4L85OBlPMsWcOTejA1la+DD8KI1p8b6cY19S8DQuPIKaDU2B/c2FRyZBBgwf2H5B96CjoL7gdEWUV3hOT+qDV6jo7VXq94fqN28OGDP3tt2lgXbZnnkJjCo04AjWD5rpuvKLPG0UvZ9509ijpehCVA+nvTZU0HHZzoEGuWlpaS0rLyysqb9/JL6+orKio1Gq16KSgnO3W1jbcZ3Ax939XbeFX5YcKWws0FklGjMUhJYWWeW+VHFoFNObSl0lQOdnTCe0BGkEQ0jOylnl6Xbp8tarqDV5y4L3Kd/+BwydPnRs8cFBYeMT793XENHviTWtSeOQCiK5Go9FoNNXVNZMmTTlx8qy3t8+Nm3dsK5GYaBMM13WzJUftWORNfoak6/oUmrcRGR3FGNLfQCNGGYdnZicR03RXEAS93pCekRUQGDx27A9Llizr26t33169B/Tr//2YsbNnz83MytZoNNbCDZLMVkl5ch7QWAxmrsnEhmEmFj7TixSSYZRk9+nJInTK/xTHZUr37l1dyLowuAghIXHHmze1B7Nz/NcE8jy//8BhX9/VO1J2//LL+PSMLLVaTdtW4Rn8bsA6o9FoVvn4ZR862tTU/Ox5oZubR1tbu/3FZxjGaRSCCx2SNgCj7KNeYzTdMm4nV2LqgSwS0zxN6LoY5vAs7SE0tm3aHOfj4xcWHtGr55cjXUf2/sql/3/69nHp1avnl31cevX+ygWOPiU2mdDhGGD8aRvQtLa24ZVd8F4oMr8AACAASURBVHND1Ea8KZm+el0mQeVAI34jCQcMuDAdVJyUuT4g0zfoHiXOy7ErGuZ4U86tZHS6CK2tbbFx8YIgVFfXjPnu+59//tV1uOu9+wVarW758hXXrt/alpCUnpEVFLR20aIlHR2dCC5AarVao9F0dHRqtdqz53J//vnX6uqa9vaO4yfODBowsLyi0r4KYEcO2h2Gl1rzhjDoU0O7EaM3jVOOiaDZxdEPtS+H52cPIW979x0YPHDQhAmTBvTr3/srl95fuQwZNLj3Vy6AMr16ftmr55ffjxm7I2W3DaVgDgkWKBtNekYWfbecWGZooIG7MvLyH9A/AwKD8fQJ+4FGXtSZLkh/MhddEggkc5FcF2MYkMxXkpNPQJKFlQzG1N6hw8eu37htNBo1Gs3kyb/NmjVn3rwFzc0tL1++mjZten39h5270rMPHW1ra0/duWfZsuWnTp9vb+/Q6w3gONPR0dnR0dnW1v7y5as//vjzQcEjjUajUqnmzVvgOty1ra3dgZWAZhdcz0G5pt8gDGFgQq2aoa3WsfQ30DAal+Bo672j6MbNO6C8ALK4fNGTxpev+/Yb8933q3z8CotKPD29njx9rrwUcOoVXqKC78FIjJfs0EeXMykg0MChNmhRhvPl4fQsTJM+ucZcgjQp+UqrErzIE8ocIWqIsUAcXR5fmJ+YgkL8UpKsTDCm62JERj1nQkp+hQetVjtzphuc111cXOo63LWurl6j0XAcl5CYHBEZ3dbWfujwsYTEHaAaPHnybNyPPx07fpozHYjV0dEJuw381wSeOXsRLDXpGVmTJk0Z6TqyoqLSUVJGuvr70o4FuCBFQwzoNbRHC753io1GnG43BBq6E3h5rfy6b79ePb/s/ZVL3169AW56f+UyoF//Xj2/3JGyu7q6BnyoCotKfHz8lG8qyct/gKtOcHI9w0B1dQ3ADX2uPU24Os7oRHATC60N2QA04uZnOLRNR5BJRHIyZTEpSYm1py8piSvOgsEOMWM0b+LoIJNnz+WmpKaBlB4/cSZ47ToQy8bG5okTJ1dX13R2qvbuO5CZlQ2L3AaDsbq65sOHhs5OFUCMVqutr/8YFh7ht3qNWq1ua2s/dfqcm5vHi8LijZtiUnfusblaJIk2DzFOKjilIqYZE2fa4Yh2JQzjWK4E8VGepOu+7e6ANTQnbW3t4378CdQZABpQZPq49BrYf8CUKVO1Wh1amniezz50FG/wUkiw1E3fqcJ8hbsBBdH5L4LpMhYwxEjCCoZXaKOhyZxSIDkqSE5tGAETp08vjhLzB0Ur5Nli/3FI77KYiHw90G+YZ6PR6O3t8/59HRhcEhJ3JCXvhGH//IXLEZFRGo1GrVafOn1+c8yW+vqPbW3tnZ0qgBiVSqVWqw0GY2Njs4fH7IPZOe3tHc+fF65Y4R0UHFJV9Uaj0Vy7fmvX7gzHihitsNDmXtLVg4ZeDkOgofciOJAloB4ILoJI1RQc1BXsIWbkeVDwqFfPL0GR6ePSC2ZMgDh9e/VOSk6l56KEkNrad/7+AdbmKGP9ra6ukVlagk95+Q/oA0B5nsdbXMRAYxVjgtQILCnPMoMSHZieNWC3wzSt1Wjk87ItupIUmKqQBBGm1OLodE+DqlCpVBs3xRDTSo2X18obN+/AriVvb5979wt0Or1Wqz2Sc2J7UurHj421te+ampp1On1HRye4pdTWvps/f2Hi9hSO49aFhvfr3cd/TaBWq1Wr1Z2dqqqqN+sjNthfS0xZ+K7HdBLKKoKLTYQQPDudUEtRXNdTHBxI7C0IyC7z8LkI+wQ4RB07fhrmSoAv8IA2msysbNoXkxCi0Wj81wRa3I2al/8AjTKtrW2g0QiCQAg5knOC/gTGlz3pmZLpIAbB7AmwhphuoTNno1FIVrWFwhakFR96Vs8Iqm1syMOE5CerElf+SRJoxPiCBNXy/Hnh1vhEnufhcpXff5/x8uUrjuOePnuxzNNLpVLBMTQ7d6VfvXazqan53bu6+vqP4Jj38uWrEyfPurl5rA0JPX/hsq/v6g1RGwsePm5ra4eI4CK8LjTc4SJGul54QJeLHoNpjxv0D+a7+hY7kHrQjoOCqPY/IzE8gOFq5650BBcwA+Nf3169Hz56gvMmmDNrtTpfP3+VSiWfV0JiMmAELEiDFUagtBv6E6oq4iqilR3EGviJ55wnJCajXVmciOSYLFNF1gZgRhT6vYzxmGaJ4c1cFuKQShi2yL/FlAk1cJoLL/nMsE0I2Zd58EVhMfjdtbS0url5gFU4JCR05650ACCtVhsbFz9t2vTCopLyisoTJ8/u3XdgwYJFI11HjvrvqCVLlkVERsXGxd+7X4ATE9CJwPcvZF2YQ9aSJcvL+OMRylosmIxQ9IyJmLnFxSHUg1EBug/QCKIDt9Rq9eEjx/v/py8YaGjVpvdXLoMHDmprawegefny1YoV3nDtnq+fv0W3KFiiwnu1AWWALuZeobdBBQQGt7S0CmaqiL4jQTCtPW2I2gh6TUJisqQfjXJxEszrGjLtpaQ1iWjLL/PVXOeTAUpxUpJzMZmf8oViMsUH2sgoDsPEFS85oYVi46YYrVYLa8ANDU2TJk1RqVQ6nX7lylX37hfwPA9u6KFh63t/5dKvd5/eX7m4fNFz0ICBw4YMHek6Mnx9ZFXVm5aWVkIIDJNYjbzp4IjQsPWwJ9NcMRWSTCvQ602guWCRYVMFTxFMnZxyHg3afrCFhO4ENDQbRqPx1OnzYKDBxSb8D5Zgg8F47nzuH3/8mZ6RVVxcqtXqFi9eqtcblEiaxTcKCTu9TADQjwQr5xdi4VHOj8xX7JFESh2wKk0bgIZJkK49hZYmcwkyYcToI4gaC6uipubtutBwvEL7+fNCD4/Zer1Bq9XOnTv/3bs6g8GoUqn0esOyZcvnzp1/+MjxrfGJgYHBYeER6RlZz58XarU6juPUajWc8gm6DAo8+PIlbk959PipuTLaTES02MRsiYCvcBwXjUd4Ya7DWeohmNZNcRwQug3QkK7bLgghhUUl/Xr36f+fvug+4/JFz4H9B/Tt1dt1uGtZWQXP8+7us+7m3auurvlp3M+Vr6q8V/naJjkyYzhdVwoTpBehnr8owqUryaxluBILmKTk0D/FI7m4lbG3yZQLw5vrHuIEJbmVjMuJDgA0VxaZdJjcmWCSao65msk5erKwqIQ37TZMz8iKjYs3Go319R99fVfDrgK1Wl1XV//LL+Pfvn3Pdb3kBKckINVqtZqZpHAc19mpOnzk+ImTZyVr2wYiFKHqBMqUVqsDWBFMhwRypp1NhLL6cyanYUexhNSDNhfRjd0dgEYQLSF/+NDw07ifQYuBRe5vv/l26OAhoOOkZ2TxPF9eUZmX/2DOnHlbtibcuZsfGBisPDtJsRSHkQxg7icxGYPBLRg3Ipg7a8JcdrYFkJcr5llyzBfMqwMW8xInblUp5BOUARpBhHTmgE/8E4LFxG5tbm4xGo2ghqwJCHry9LlWq31RWLw7bW9HR6deb3j3rs7NzWN32l6tVguGYVBV8JonQgjqCFB8nLmAcnQwOwd9x+0nce/leR58lOkLwtE0g956CDSo7ziKJaQedAeyKGOfnpjOodXqlixZBhADs+LvRo/p26v3iGEjRo8aPX78RK1Wd/Zc7jJPr+nT//D18/f1809JTRP3UZnsnFEKWK5CG7CnpxeDMtZKoGQAGSBQAqDmksKx0RxXFhGZJps7sQwuyMcS44tkfyCUHaq9vSNyQzQM+1qtDizBYJFJ3J5y4eJfGo2mvv7j7Nlz/dcEajQarVZHT0zoVWQ4vAZ3LfKmQ2pA+Hen7X3+osi2CpEnHBvofQYCBUDIJ1qIOWqzpcP56cF1PSlH3DCfnRhmDh85/nXffn1cesFGp19/nfD9mLF37uY/KHi0OWYLDCYfPza6u8+K3hjjvcq3vv6DOBFxFtYWme6v4sFThn97MjWXDvMs5oRmVT4d/M/41NADnYysyvyk40pywryUhyS6aMyiAROSWUZhiiZIdfvyisrsQ0fRT7+wqGR9xAaDwdje3hEVvbm0tNxoNK72D+jV88u7efdwWxOhrpRFSwdvOpsGRZozHVij1xsSEndUV9coNLTLvKS/AvGmhWr60BnMCDmhPfc4alOCTBa2UQ96sZ03v8ApUzCH8yRPNTVvfxr3cx+XXrD8BHtG3r+vM5oIStTY2NzW1r4nPfNgdg4xv2hiMylP09lAoyRr5SBoLqTCN0q+yhTctgoRQy39IAYai1fZJe/YdePmbZA9vd5w+MjxU6fPtbd3NDe3TJgwqa6u3td39ZIly2DnAQgnPUVCTCFdnVl46uhMOKV8bUhoZ6cF3wsbiKcI163B2AQBUIXhqZ0HOO9z1tQJTYA2AM2nJOygp06f69XzSwCaYUOGft23X17+faPRqNcbtFodTjiNRuP793UTJkyqr/8o2KS0y4ilPeClRL8Q564wWcmfYtUGfor1ZCYWQ/LJivlxFDYp+crkiNzyogVsY9crzARRoZYsWfb+fR10J0JIVPTm2tp39fUfi0vKpkyZGr9te2xcPMgtqDOw8QUHOTwjglDnS/GmZR3QDcFnz2uFt8UlURsGJMQ1ZACgjTbKYBg83hi+OtFGgz483RxoBFMNqtXqlStXwc6DAf36Dx44aJmnV/aho2q1WrxzLCho7YcPDTarD+K+S3+yLTWF4qdErsyxKhndWmhj8Mgi20rKJbb10NVrrrZpOKAhT8yAuA+LxUay3vBlY2NzWHgEIIJWq1Or1esjNsCZMtdv3B48cJCbm8e7d3Uw9wENBQ00OCVBYzDaR1CSeZ4HCLv817XE7SmCJeJ5Ho5GtxiSLhFODznqAGN6eZundirQ0ygn2mi4rq7KwifR6m0jZEyn04esC4NNlePHTxw6eEgfl16nTp8jpk0cHMcVl5RlZmUvWrQEDluWlwobJFBGZiTjygCWOWZsG8rMfZJ8sCjegmj2IXR1hpDhRKZo8i+JGYVRUgVDHdZciWicYnIU18adu/kHs3OgF2m1uhs3b6fu3KPRaKqq3ixYsCh6Y0xjYzOsFsOFcIx/Ctw/Cw/0niOciMFU6+mzFx4esz9+bJTk8/37uoqKytxLV7YlJHmt8J4yZWrBw8fmqlpcdTThfA0NMcgeHHrLdb1xxVwb2Un/2+vEUZsgBNn++hmJ7nnXb9yeNWvO0MFD+v+n7+TJv337zbfTpk1vbGwWBAGM/Hq94c8/3b29fR4+emKz3CIpFA+FcZk38vMXhUR3LBnUkBQ2i5yLzRzmsEmQ7TwyURRyIg7Jd909IxlXjDVENKVCW0byjl2PnzxD44vXCu+S0nKNRjN37nzYsQ36iMk/RYsHBoAKgx7AqMug1QN8/GAr5u+/z3j+vJCYRiwogk6nLy4p27U747ffpoHTRq+eX7q5eYz676gzZy+aA1+Z8mLiOJujl8ZoVnnTBZUKc7GW/nclLjMmdE+ie0lU9OYtWxNSUtMWLVry7Tff9uvdJyFxB2c6iPDe/YKKisrff59x7PhpOu5nKZ2SWnVUzUumYxW4SEZkoNDcTEo+FxvKKMYXcQpG6lQQc4koIQhpMBi9vFbC0RB6vaG+/sOKFd4vX77y8fFbExDU0dEJF+DiScAANIQ6ChNsLvQ0ip5PQdyt8du3J6Vqtbqmpub7Dx4eOHhk0+Y4v9Vr5s1bMHfu/IULF8fGxR/JOfGg4NHjJ8/a2toDAoMzs7IV1iFTKGQAnYNprgi1AYpeOLOqmZTQ3/c6IZcOz8PhVPmqauLEyeBPBb2h4OHj8eMnHjh4BCxz6yM2fD9m7PChw/YfONydS0TLj/180okwzwqjmAtvLZ/mgMaiucQib+bSRChkxEwmccaaAymUV1RGb4wBHAFEyD50dPHipVev3cTNkEbTqcDop4drKRzHwXIEMW2JRmsIuPPV1LyNiIweMmjwn3+6e3jM/v33GX6r12QfOnrufG5FRaVKpSImTwKTuqQ1GIxHj51KSNyhpFxYHELtKTF2PdfK2PWcYMRE5xqDCTXFFbq3UsObNmiEhq2fOHFyUnJqU1OzVqsDdfTGzTvDhw6rr/8IOO3vH7AhaqPMdkr7u7iS6JKflECADUQLmzwb5vihX8rHkhmclGgWvCWPLaaKxBwy4Zm5v0xxxJVDv8nYu//qtZuwqvD27Xt391n+awKTd+wCew2oM2BnQewAowyoDLxpyQkUBNAR4PhOg8FYW/tuxoyZvr6rs/Yf8l8TeOr0uY8fG5ExxC+8YgnMKFqt7sbNO2tDQhX2FqZcaAPmqDOuQG2hffbwAUqhJCOrqAfCnmSLdjfSaDRh4RF70jNv3c5b5uk1e/bc9IysyldVla+qdDr9uB9/yst/cOdu/pWrN37/fQbYhu3JztzwKPNeMFOHdPObi6iQJXM/xSimvGtaVVEYnliazzMVYo43cwAhKKsZcanNNQH9FZ9p75KQdWHFxaWwNWlr/PZVPn7Dhw6rrq6BnU0wUcJ5EyoI8B8XuYHgJ8dxoJgcO3566tTft2xNUKlU8BJDEtMyMw0KCARarS730pUJEybBsQEKCUuHsEX/R/Z4EwHMYXGUZ6SQeoiHQYfn4SgihGRmZcPRnNA2N27e/vXXCYMGDBw9anTO0ZPu7rM2bY79adzPo0eNHjJo8Js3tTZkIfnSHNZYlYhMavJx5ZlhxEYhG5KMWWRJXAnmVBsmWYsRZXKXjGsxfTo6Q/AJpwxoBG1v71iyZBlgikajWbHCOyIyKihobWenSqvVwSwJ9ijBUVi0doOL3ABAMMmCnx8+NAQFhwwbMvRi7hW93gAHgIK+A9Mx4ASj4AQNYEKj0WyI2jiw/4A3b2oViiehTpZBEwxdbzAvY8KAB/MnstF0Z+J5PjAwuLikDKoGOP/woeHGzTtpe/Z5e/t8P2bsrFlz4KyzsvKXvH0eAeb6Lv40Jx7mgMlcUnQBbWZVSUkZEWWYoSVQYcpKAEJJYa0CGqErfIjLQr9nQtL/6SHWaDS+fl39/Hmh9ypf8J3JPnQ0LDxi0aIlzc0toMgArOj1BpVKBdYZ3BjNuOfBT5iD1Nd/9PT0mjNn3vMXRRDdaLrHEo3KaGaCZ73e8OFDw4vC4l27M5YvX/Hnn+7Dhgz1W70GLDjm2kKyilBMcK6KHKLpl1BL4BbN/DZTD7GXZLellpbWjL376c4Eut/793UAz3fz7n03esy+zIN4apkNMGoOEcz1ePEbGQySz84ZIwmTlzlkhAdxP5ORf/pB3IUs1pVM3SphQLI4kpVPdxh8hkH+6rWbyTt2LV++Yk1AkIfHbC+vlYVFJTqd/mLulXE//hQVvensuVxQQGCmA2oL6iO4SExPgjCkwWAsK6vw8Jgdvj7y48dG0INwYRRj6fWG9vaO4pKynKMnk5J3rly5ysNj9pw581auXHUwO+fQ4WMFDx9XVr7G2yOV92dEFiw7rcThjA/P3KEXpBRmoZx6GKn9mt0caE6dPnck5wTp6vjDcdxq/4BHj5/Cz7t591yHu8IVGUoKJS8PTO9kHiRjKQEjmeyUh5SXQHOcyL9kpFQsxjJGXHEtif/LpGxVvUm2kSTKCKKGw5+trW2DBw7auSs9/96DysrXra1taHnZnpSalJzq7x/Q0tLa2amiHdtg7oOuMTx15QDP82Aths759u37adOmz5+/8NDhY6AQwcwItYzS0vILF/+Cy3YnTZqyJiBod9re23fyz1+43NDQhBuy5BtFpooIpbgBMa6D8KDRaJhSKMzCKupyC0I3JCyz0WgMWRf25k0trpHhg4+PX2Xla8FUuYePHA9ZF+aMyhKsaWZz781hhMwnezgxF0smL7GgSka3IXflxLCnJDtJuJHEHQCCK1dvzJ+/EA5/QDe2lpbWZ88L1wQEbY1P9F8TiLBCqKPqADUYJxQ0c4CGcjH3ykjXkYnbU6I3xuTl39dqtS0trUVFJXfu5u9I2R0RGRUWHuHhMTssPOLM2YsXc69UVFR2dqoccn4wU2l816tvkVU4VBvxBY3ETkKD/91U2W2BBunNm9qg4BAEZkLNPB8+egJOU4IgGI3G0tLyKVOm2rDbXWFvdlRS5mLZEFe5WNoJNLbRJ+tdYqxBYcNhCYZxlUq1ZMmyCxf/MprOx21qaj6YnTN+/EQ46H740GEnT51TqVQIK7jrGiZQaJThTbsNcDUqIjLqm5HfeHv7CILgtcL7xMmzwWvXzZzpNrD/gFH/HTVzpltsXHxJaXlxcanYlO5ABMcEaXswwo1Wq8MVNBorSddjLR1FPQTFpsTPSISQvPwHWfsP0eoMsF3w8DF45SEG6XT6OXPmwc4D5UUjUoZS21j99PXJ5KhEsK1l0p4SOdv2JEmSqg0+376TP+7Hn548fZ5z9GTqzj3h6yOXL18RvHbdvsyDhUUl167fSkpOLa+o1Gg0Wq0WZxkANGjmQNhCoKmpeRsSEjpt2nTX4a43b93V6w1R0ZsCA4M9Pb22J6UeyTnx6lVVY2MzGlyc2ltooCFdDcMANLjxCkduh4MdUg8npetYIoQcPXYq/94DQTTl9vXz35OeidUEA9S+zINBQWsFK4vmwCa3OR2HMND9G/TTEC05nZ2q8orKBwWPUnfu2bgpZntSalh4BHj65+Xff/nyFcxcILxOp8/Mytbp9CqVSqVS0UM9bebAB9B63rypXe0f8PDRE09PL29vHzAhp+7cw5k5HcHZzUQo7VUwdW/UXBBl0BhMmz4dzkwPJ2lKjiVCyLaEpA8fGgSRTXHevAVnzl7ELsWbTmadOdOtoaFJ+FRSR7NkT1OJlZF/Lmp8es2OIYPBWF//8crVG6dOnw9eu26k68jJk38LCQk9eeoczhcE0bIUIeTt2/dwvSTcbItrNOgpQ/u/EEJgRWnmTLeCh48JIQGBwX9dua7RaJqamnen7RXXA50j/UZwaHMz5cJJAC5mw24Jel8CuvA5igekHqgFdNsODYxtjd9OVwFWXOrOPXC8K8N/8o5dmzbHdn/b078kSUp6Iw0NgiBwHNfa2vbseeHtO/lnz+VuiNoYvj5yXWj4xk0xidtTzl+4XFpa/uFDg1arM5cLpnbg4JGCh4/BbU+lUuGyNPie4CHkxHTKDCEkIXFHVPRmg8HY2Ng8Y8ZMWK569aoqa/8hh1eObYS4g4oYOjejVRhdaRyee3d32IMy6/UG9KDB98B5Y2PzrFlznr8oIl2pvv7jpElTlDtT/kvdisxNLuj3arW6sKjk4aMn5y9c2hq/PSAweEPUxpjYrVn7D70oLP7woaGjoxNXW2TSBKJ9iGJitzY0NMHdtWAxRVsvDvvGrtsRyysqwbnm8JHjMbFbYdpVVlZx6PAxZ9aTBaLLDoTuLPQ+CdoPiDjJGOw8X0BHESGkpLScVkFpJZAQcjA759Llq/gGFdpNm+NWrPBub+/43CX4l2whBhew6VUqVV7+/YPZOZ6eXqP+O2r8+ImxcfHnL1xuamqmRxrGIMI8MNqQIAgcx3V0dJaWljc3t2zZmgD4AqtORtMNKnjqJXPHIxxSA3ZiD4/ZZeUvwYqcl//gxs07n7LSGGJKypsOzcHZEzgEoV4jmBbmHM4JCzTdE3Eys7Jv3LwtiMxaUClPn72AM1wFCoM4jquurvlm5DcJiTs+M/f/kh2kVqsbG5sfPX565uzFTZtjvb191kdsSN6x62B2zq3befX1H8DQgEsqgmgYx6TEeg3sNnj58lXO0ZO+fv7z5y8c9+NP8+cvzNp/CLYd0IdagYEGjTU85WILAKTT6W/cvB0UHGI0GuGCyp270ouKSj5PxXUlrAeUGoQbXnSmpzNAoEf3V2cEQdi4Kebly1f0e6iXJ0+eqVQqQRA2bY7Ny39AqEPnBUHYnbb3t9+mZe0/1J0L+C9JkkqlevrsxfkLl318/Ea6jgwKWpuZlZ1/70FTUzMdTIwjzDNjFiCEwAFGN2/dvX0nPyp60+hRo7/u22/GjJmBgcFxW7bdvpMfERl9/sIlWNXGHdigwuDRM7gpCScg8NJ/TeD5C5chllari4reVFv7zpn1JEeSIEuDMhSB63qgurOuW3F4ig4nnufXhYbX1LylXwI+JiXvXLBg0fak1PMXLvv7B7S3d+D5Zi0treN+/Ckv//6LwuJbt/P+xZpPRkz/llQrhK7KqSAIOp2+pLT80uWrW+O3p2dkhYVHREVvSklNO3P2YnV1TWenijFSmkuH+U8IgcveCotK9h84HL0xBjYTLViwKHx9ZNqefVeu3qisfN3W1g6mX57nExJ3vH37HpaWcNOAkTpVFwlkEjZY6/WGlpZW/zWBLS2tuP0yKDiEtj1/RqJnT7TlgVFtcDO6wxnoIalkdisyGo1+q9dotVr4ySjGjY3NN27eaW1tWxca7uvnr9FoYDAJCloLq051dfXeq3w7O63Y+fov2Um0tOMbJJhlNDQ0PX32IvvQ0aTk1KCgtRGRUUnJqafPXIAL1PH4JToinTjzgIOwXm+or/9YWlp+MfdK3JZt60LDV/sHeHp6hawLKyoqKSoqqa19Bxfa0ozhs0qlioiMwk3V+IBaDN/16BY8wxwcUmAdR6vVwZ6DsPAIZ1e1VUSDi2CaFvDUrZUG510gh9jm8KQdQmD8CwpaiyhLTFsNBNO5atDkVVVvfv7517z8+zzPHzh45JdfxoMZ2Gg07knP3BC1EZSdf+HmkxHWNvauxsbmwqKS2Lj433+f4TrcNXJD9IWLf8FCsiBlQ2FsLgIFLpzpHkgUnpLS8nv3C7YlJE2bNn30qNFBQWtTUtMuXPyrpuYtusygmZO26SBxHFdV9WZ32l68LIU2x+BFArT1lKM2QMMhLyqVCvSCly9fxW3Z5uxKtoqwrugJFK5z4wTKGVn3wEHGGanbT4SQjx8b14WG029oQn2P5/mw8IgpU6Zeunx1xoyZHh6zT546BxXa0tLq4+O3QnmPPQAAIABJREFUaXNcN/cY+v+JQAWorX33orA499KVlNS0+G3b/dcEHjt++uq1m+UVla9fV2u1WqYtxEqQIKUfcRzX2amqrq65eevurt0ZgYHBMbFbQ8PWb9ocB+cq1NS8hXmQeGJlTkWC/4ePHL93vwD9ZXElGId6GoDoZW/AI7VajWdKHMzOOXX6vLPrWTkhdjNTJ1RneOoYMIdTD0T6bit+xcWlkitH2D/QHzwiMmro4CHfjxlbUVH56lXVhAmTwFNTEAS93pCUvDMlNa3bQmr3J4s9xGAwVlRUnjp9LnF7SkJi8s5d6ekZWafPXDh2/HTlqyq1Wo2Vb07OzT1otdqXL1/9deV6ZlZ2UnJqRGT0moCgHSm78/IflFdUNjU1azQaSfZkgEwckuf56I0xcI4njvxQLly9Rj9aRgvAE61gOwIhZGv89spXVZYq9VMTQgz8x1LglMq5xmDeOe6ADqG7efdi4+LF77GD4sqcp6fX92PGJiTuAK+H/QcOz5u3gB7K/FavKS0th2r91MX4h5C5FWKe2q1DQwDHcU1NzU+ePt8av/3332e4uXmkpKadPZcLV6OJ1Qehq1rB5E5nx3FcW1v7i8LizKxs71W+EyZMCgkJTduz7+mzF2/e1La2tllVLqKAqqtrfP38Oeo+AFyRAZQhpsMiYLpBH7KLC+F4OLn3Kt/m5pZu1dPERUbFjXYRdhbQmGv17kCEkPKKykOHjxEzWjQKgNFoXObptWKF95w58xoammCtYdyPP8FmfOgTLwqLly1bDobA7lnebkWSVaRWq6ura+7dLziYnZO1/9COlN2bNsfuSc+8/Ne1ktLyxsZmc4MWjVxiRYMQ0t7eATunk3fsioreHLIuLDRsfdyWbQezcwoePm5v78CFHhn2lBTKHA+nTp/fnpTKUWdToQQi0OAbsMhwfx8hroVJB5iE29raQ9aFwRWp3YrosuNcCQXEaLr0zuH5/u8COaEbH0lT8PDx7rS99BtmeBRMVbZ48dKcoye/7tuvurrm48dGo9GYlJy62j+AUPfkhqwL++vK9W5b2M9LhFJVCKXICILQ2al69Pjp9Ru34Z6zdaHh9x88rKp6o9FoBJNeibHoKZL4J+l6GZNWqy2vqDx7LtfDY/a0adMDA4PhoLmGhiZ6qZFmzBkKOMdxW7YmVFfX0OoM7UGDNlRmjQaMNXgVNyw51dXVg+dedxvPsI0IdakmIQQXzpzosMfow92Nrly9ERsXL8MeDj7+awKfvyiaMGHSi8Liurp6OIB+ypSpMMzC4a/v39et8vFj/L7+JZqgPuvrPxY8fHz6zIXdaXu3J6VuS0hK3blne1JqaWk57DNkkIiOTusLtCIjCILRaGxsbH7y5NnpMxeSklPhrLmw8IjkHbvu3S+or/8Izm/i6IKUPuvATstx3OaYLTS+gNqCQz29GAzWDc506hXYZXCDgtFohHuBuuF4RgMNEGpk/xc9g2mW/rpy/emzFzLBAJI7OjpnzJjZ1NSclLzzwMEjnZ2q5uYWjuPSM7JSUtNAeMDLJv/eg3Wh4U6yrn9GsnkqodVqm5qa6+s/PH9eeDA7JyU1LSIyOnnHrrPncu/dL6itfQfWTXEWMlMkfFapVFVVb/LyHxzMzomIjF4fsWFD1MY96ZnXrt+qrq6hXVo+L12/cXv/gcM4iaDvb4IzouCiFZw3oSstOPWBXlNUVLJpc5yv7+plnl7Tp//R0tLaPYULCdGTXq13oh+NuDo+YwUxw1fclm3M/gNxd+c47tWrqilTpnIcd/7CZRhM2ts7YKjx9PSClVScUS9atAQWpLphP7CNONOOOFy/hPfMvJgezVQqVXlF5bHjpzfHbJk0acqCBYv8Vq85ey63vv6DjB+AeNpCqzYwHnZ2qhobmy/mXjl85Phvv0374Ydx7u6z1kdsqKx8zYtcY7oJRUVvyj50FKwqMMKbbnHSweUqsPUJtDlc2wafYI7jtFrtufO5337zbfKOXdOmTZ81a86QQYOrq2u6WzEF0T0zzJQQJoAOz9SsRvN5gQa5MhiMoWHr0RBgLjzHcVev3fT1Xc3zPJw+D9vt1Go1IWTjpphjx08Tk/sDx3F5+Q+8vFZ2Q1udY4nW+IxGo0qlKnj4+MzZi5lZ2Tt3pUdERmfs3Z+SmlZaWl5Z+RqGbjqKfLICZTGBWWpFReXxE2dSd+5Z5eMXERkVvTHm9JkLDwoegeFDcjbUTYgQEr4+0tfPP2Rd2KXLV1+9qqLNwAA6cIccuMnAoeWAO2q1+srVG4sWLZk50+3M2YuEkGWeXplZ2cuXr+iGNhpBtLRHqzagrDnDBaQL0Ng2+zWnE9lMND+1te+2J6VKssR09z3pmW5uHrDVYG1IaPy27RzHtbd3qNXqsrKKsWN/gAP68EIMT0+va9dvka5XiHTDbmEV0X0IS9Ta2nb12s3YuPilSz2nTJl6MDvn3v0CxtQqttPRL5nKQf1Iq9VVvqo6mJ0TGBjs4TH7559/zczKfv26ur7+IxPY3GDWfSoc0OTS5atTpkx1He4aGxdfVFSiVqtB8OD+7I6OTgim0+nhTUtL65GcEy5f9Bw0YGBZ+cvOTtWu3RkjXUdGREY9fPSkGzpS0DovR50xSFugnAg0iGo0Q0qYJl2dmh3LnE6nj42Lv3nrrrhHMr2fELJrd0b///Q9f+GyIAivX1dPnDgZLsdpaGgyGo1BwSHbEpJgBg5Ac+z46S1bE3C7Cr1o8g8l4L+jo7Ohoen+g4d70jPDwiP2Hzickpq2L/Pg+QuXXhQWv39fJ646SZAlJtutVqtrbm6pr//Y0tLa2tr26lXV4yfPEhKTExKTo6I3p+7cs3ffgZu37lZX14AzrkCBlGAeTejcnV0zAiVLjDGCGWZA73v58lV6RlZU9OaAwGBPT6/E7SmPHj8tLS1vbW3D1RlAnDdvar1WeB/Mzpk/f+FfV64v8/RasGDRjBkzU1LThG6mtQHRI6vRdNIVoU6ocZZGgwAh2ds+I8EJ8mDHNScMgolto9E4b96CrfGJHh6zYbqUc/Skl9dKPOS1paXV3X1W1v5DYLojhKhUKk9Pr9evq7tPkRUSoVS5jo7Ourr6srKKzKzs2Lj48PWRsXHxawKCwLHt3bs6hfNtcd3yPN/S0lpf//GvK9cTEndEb4yJiIyOiIxKSt5ZVfVmX+bBh4+eiFmSefN5iXS9jpr+KdPzwWBx7fotD4/ZixcvHffjTytXrip4+HjvvgORG6KDgtZ+M/Kb6zdu19d/GPfjT7/8Mv78hcs6nf5Izom0Pfu6Ww0AMcgiUOoCHlfuFBsNM/J0k9ohhFRWvvbyWonqEvJGmw9w5Gxubpk4cXJTU/OUKVPB95fjODc3D9hjCWcjlZW/HDFsxN59B3BqeiTnxK7dGZ+znF0JC8i8ZCwmhJDOTlXupSu70/bOn79wypSps2bNiY2Lv//gIVhb0SORaU00GDPATcsbLGyfOXvxYHbO0qWec+fO917l6+8fEBO79a8r11ENQWvO/wXieT5uy7ba2ndFRSUJiTu+HzO2X+8+vb9yGfPd93fu5oMisHDh4pTUtAcFj7Ra3fkLl7rPUcEMYSvTjc6ZtobyJjdoh+fbgzZBd5+uQwg5dz7X3z+grq6eUP5dzIQfvRtevnw1f/5Cnuc3bY5Nz8iCspw5e/HPP907Ojph4YDn+bz8B3BUPcD5s+eFy5ev+OyzaFrmiRRpNJp37+pKS8tPn7mQkpoWFb05NGx9RGTU6TMX7ubde/26GhbymXSY9PFZECGaSqV68vT5mbMXd6Ts3hC18fSZCxGR0bdu55WVv6yoqOzo6Dxw8EjW/kPHjp+Gbdb/pwhq7/Jf186cvQhjflXVm/SMrCGDBm/cFAPmG61Wt3NX+p70TI1GYzAYT5w8i4bF7kZM18K1baPpyCtYaHN4vj1w2fwzAo04X0II7H9dutTT29snPSPLSJ0yzfP8x4+NhUUlB7Nzsg8dTUreuXFTjL9/gNFoPH/hElj7AZVCQkKPHT/N8zyY8Qgh79/XzZu34PCR47B24OPjV11dI8nDJyOm5nme12g0ZWUVBQ8f78s8GLIubOXKVdEbY2Jit+5Jz6x8VdXW1g46mjiuIAUx9Bu4ZKOm5u3F3Cv7DxzenbY3Ni4+IXHH5pgtt+/kFzx83NbWzkBeUVFJSEjo8xdFe9IzyysqJbHsn0K28UwI+fChIXx9JJwirNcb8u89GPPd9/HbtsNqlE6nLy4udXPzaG/v0On0MB44nHk7iYEYwSRlSGCdgdmTw3PvIVanHZ6HRWLypTt6a2ubm5vHlClTwbxy/8FDcFQd6TqyX+8+M2bM9PT0WhMQNGLYiN5fueReulJSWj561OiamregqZWUli9cuBjn5KAc7tyV3qvnl7fv5BNC8vLvb0tIEj6f2KBGCWdBwX6LVT5+340eM3/+wuiNMY8eP21v72BUEtqMJ3TVU+hg+EavNzQ2NldWvk5ITPbyWrlw4eK9+w7k33tQWloOE3LaiEu6bhE4dz53xQrv1ta2EyfPSt5S9E8hGzjHKBzHbdoci5ubDhw80sel17rQcJMjn06vNyxevLSwqKSzU3X9xu0DB48I3QmL6a5CD9joPoMGCmc57OFsTfh8Sg1vxgdMEISmpuYJEyaVlJYHr103Z868FSu8ExKTg9euO3nqXFFRSUdHJ8/zp89cmDdvQULijlH/HbU1fvv06X/sTtsLNajRaCZMmATBkF6/rv7tt2lLlixraWlta2v39fOHM7E+calhcfThoyeHjxxP27MvckN05IbopORUOAvqzZtasdesJJNirIHuUln5Ov/eg2PHT0dvjFkXGr5la8LOXelwYsPHj40KOxMhJG7LtojIaJ1OX1FRGbIuDBTDf6heYw+3G6I2xm/bvnffgdX+AR4es78bPQZ6DqCM0Wj08fErKiqB4XDT5thuhciMOsN3PaKcto6DauNwBnrwprN8hK5o9ylJZjmturrml1/G19XVC4Lw+nU1bsTA/0ePner/n75h4REw9np4zB4xbMTMmW7gakUIWbZs+du37/muDrJPnjz7um+/9IwsQRAiIqOePHkmhlob6oF0Xdal9QJ8yXFcY2Nz/r0Hvn7+f/zx5/z5C/fuO1D5qgrQkElNMll4EKMzz/M6nb6y8vWhw8dCw9Z/N3rM9Ol/pGdkPX9R1NjYbO1IBd1Oq9X9/vuMrfGJMOgFBgaXV1QKon2S/xSyBx/Pnc+FrgWn9v007ueQkFBwqAFN2d8/IG3PPtiIsD5ig225OIkQXwRTJ0S4wR3baKxxhiNrDyJyeehWQFNf/3HKlKnNzS00FKK1/MzZi9OmTR82ZOj5C5ehjtrbO/akZ44eNTpkXVhpaTkhZF/mQXALRnURKneVj98PP4x786b28ZNnc+fOP3T42ImTZ0+eOldYVAJbVGxQs+n/mN3Hj41lZRX37hccyTmRkJi8O21vSmpa1v5DN27eqa19h8vtMtkxaeKz0WhUq9WVla/PX7iUlJwavTEmfH3kxk0xaXv2nTufW/mqCu6NpqPIYw2jqvA8/+pV1bgff7p1Ow+sQnFbtp2/cMlOOP5cJMO2klK8fl0dGBgMx3d1dHROnfp7yLowcBcGjebAwSOxcfFqtbqpqXn+/IWo+jmlMFaSuGVpvYY3nb8Bz04xBtMVYbEjOolkGoPjuHnzFuAt2vSa3L37Bb/8Mn7o4CHpGVm86fhocJx58vT5seOn/Vav8Vu95tnzwpB1YULX+uV5/smTZ2PH/nA37x6cHfHHH38eP3Hm+Ikz+w8c9lu95tHjpzYMfeCLXF5Reeny1di4+LDwiMgN0SHrwpJ37Dp0+Njz54W05JurByZf/MlxnEqlqql5W1pafuLk2di4+OC16xYuXJyUnHr5r2svCovr6z+IF+boccyqskDE3Wl7J0/+Da581On0s2fPjY2Lx1ysrZ9PTMzAST/TraCwZt69q1uyZBk47BFCFixY5Ou7Gi7eABP7teu3IiKjYDLl7e1z525+d6gc0pXwDXgtMhCDR2Q4nI0uWxDQ+5jh7DOS0WhcutSztvYdDcaCIHAct3Llql9/nRC3ZRut+/Gmc6QJIXCD1/Chw1yHu1ZVvSGU+wAkvnNX+patCTzPV1fX5OU/wCOyX758NX78RMzUIvE8X1dXn5f/IHpjzMyZbsOGDF2+fEX2oaMPCh7hEZNEREwiRDQ/wv/t7R0PHz3ZtTtj7tz5f/7pPnrU6Lgt2woePgb8paMwzUe/p9mQKQsjips2x8IqniAIV67emDNnnvcqX3RdF7oZ0Igr2RzR4KuwCJ2dqsDAYK1Wq1arjUaj3+o1o0eN/vChARYZ9HrDzVt314aEgnaTvGNXN1nhZnoCFp/etG2kDl131qoTofCe3vuALx2epVVECNkcs+XwkeN0hyCEFBeXjvrvqMTtKXCnF0959NH1aDAYL12+OmvWnMTtKRCAo85Pq619N378xJqatxDxzZvaiMjoyA3R587nbo7Z4unp9fDRE5iv0vVACDEajVVVb27dzss+dNR7le+SJcvWhYbHxsXDWXBlZRXMsdtMY+NLpqT4rFaryysqz53PzczKDgpaCwf6H8k5kZf/oL7+Y1NTMzMgS9ab+KsSuaJZbWpqXrRoSe6lK7BpY8aMmSdOng0JCe3o6JRkXhI9ZfKSDGxbl2NkiSkL/YkZbBTiL1D0xhjYaaHT6bMPHV2+fAXMpOAwmou5V6I3xoDK86KweMKESdaeN+oMYorGmIHRE42YdBxneQbT3PCU8x6+F2xte4Vksd//deX6ps1xzPrLteu3Zs50wz1KdNcRTIZMRJ+0PfvGfPd9SmpaZ6dKMI3VsPd/zpx5V67eAOzYGp/oOtx1xLARfXv1Huk6sm+v3uPHT4QVTWiSjo7OR4+fpqSmLVq0ZNiQoYMGDPT18y8pLW9pacWL68RFQ20CF5LFIyow0NbWfu9+QVh4xIwZM8f9+NOOlN2Vla/fvasDb0MsGpOFcvGWqWoaX4jpVoyiopIJEyZ9+NCg0+nBfN7Q0BQUtLbg4WOF+5IZmZfpTnSdMDUjZk+SxPnKR5cMSRNjbud5HjY9wUTp6bMX4A4KRg2j0Xj5r2v7DxxWq9V6vcHLa+WAfv3vP3jobFuExVagi4xCwVP3HxCTNw3OBpy1qRJ/MOsjTGM4iSwmfur0OTjKkw6p1eqKS8poRYZJkwaaqOjNvr6rhw8d5u4+a+eu9KfPXoAstbW1w90s+w8c9vb2GdCv/7fffOvuPit+23Y3N48+Lr2+HzP22fPCa9dvHT5y3Mtr5cSJk5d5em2N334k50TBw8d1dfV4GCJdFpoffEYpwsBw4GPupStpe/Ylbk9ZExCUkpq2Jz3z1OlzDQ1NdXX14nmQDXWoJK45Wb1x8zbsHeM4zsfHL3JDNM/zaXv2JSXvxOqVZ4OIgEYyIxQD+iWjdzDRzSVIJ0UHNqfCSFYOobYC0ZSxdz8MSwaDsb2945dfxpeWluPUIyho7Sofv/MXLq0JCAoNW3/o8LGt8dtlat4hpKRxBaq6UJfB8wChpHgdAuecG1d6cNTJfeaY/oxAQwj58KFh/vyFzc0tTBSsRFoRYwQbXgYFrSWEVFfXPH7ybH3EhsmTf9uelNrZ+b/zKC9dvvrnn+79evcZ8933p06fz710ZcvWBO9VvqNHjfb09FofseH8hcuFRSVVVW+qq2voNpDp9+KpTWen6t27ukePn17MvbJ334HNMVu2xicezM65cfPO69fVcOaAODWmfiQFVVyHkpIs2wgSqRFCgoJD4rZsI4ScPZc76r+jGhub9XpDwcPH7u6z4I5acfqSWYurSFxj4pLSQGPOpCKZoCRAiyNK2sjxJ0zJmbLkXrpyMDuHN52lsC40PCZ2K2gB9fUfXYe7btwUk5C4Iy//ARxVs2KFt7PPD2RsHUxBGNHAl7iFnb6vymi6DsEpq060YQ9ZFDPt8IwVJg71siYgiDnNk5ggBtUWyV4oCEJDQ1No2HqButvw7dv348dP9F7l29raptPpCx4+Dl8f2celF0yaBg8cFBgYnJd//+PHRpwQGU0XYwqiTs+YhzCAaYKmq66uSc/IWrrU03uVb2xc/Nb4xNLS8ra2dtq7F9lmJlZYEE7qRiTxT0zEYoUTKWig+WloaBrQr//Zc7mCIHh4zA4NWw+z97a29rFjf6irqxfbg82hAB1A3PUZtpnUsErFAsOkjw0hH5hhVVyBkALMhpjilFdUbo7ZAkYZnU7/oODR0MFD3r+v43n+8JHjP/wwDjoMKghBQWs7Ojpl2sJ+kpxvClRHosuOL+kTIYjJG5iYNB1n7d5mhl/SnYAG6MzZiwmJO8QdRdImynSgW7fzsvYfYka5svKXixcvDQuP8FrhPXTwkF9/neDt7RMSEpp96Ojbt++xc0hKiLm8iGkFurq65m7evUOHj8FexDNnL5aVVXR0dHZ2qqD/CWbqWegqAMx/hXVlMZh8+6KxsODh4149vywrf/nkybNBAwZWV9eAFN24ebtf7z77Mg+K5VxcRYx4i8Mwkiz5hglJBxM/I8rjT3o0oj9hAMnqYmJB+tXVNSEhoTD4NzY2r/YPGNCv/85d6XV19WO++z4peSdIaUdHZ1XVm2fPC+fMmVdWViHXVDaRuFrwv3jcZYqAphnYrk1PoHD9xLk2Gqa6JdvS4WQxZeQhNGw9nNtGV6VgqjtJJuF9UnJqeUUlR903DIl0dqq2bE344YdxW+O3o5+OuHkkfyL8t7S0FheX/nXlenpGVkzs1q3xiTtSdu9O2/vk6XP6BjXJsVrcnJKdg/7KRLGzUSSzwIyiN8b4rwnUarXTp/+xNX47dse5c+eHrAtbvHgp7T9KRPgiSPUcpibFmhcjJ0ws0hXR6AcMTKuETIL4Rugqk8prrLGx2dd39bt3dceOn548+bcRw0bcuZvvt3oNLA7sP3A4fH1kWHjEn3+6//bbtJkz3Qb2H/Dk6XPl6cuTuFaxQkhXuaD7uTgYY/flqAs5eZ531pnBglT/ZppNsLtPmyOFLc1xXHpG1oIFi+4/eIieKYgvsNuAThM5V6lUHh6zVSoVXRyMznHcq1dVYOMkXXFEoCSB7scg6q2tbS9fvkrduWfhwsVh4RGHjxzPPnQUV7WZamQEhuGT/ilpbKLjinVPmQoUZ2eRAfzPcdz8+Qt37c54UPCo/3/6vnlTC7yVV1T+8cefRUUlI4aNAMdrYgJ6OhGcYzJAgE2DXwVqqEAmGVdp1EaZsoCJjVBuGYJoYss0B+kqhFb1akjZx8fvhx/G9er55fChw3x8/AwG4/ak1P7/6bt48dK0PfvWR2w4dPjYvfsFy5evGPPd93PmzHOgjUZcIlQ/6cqki2Y03RSOb2igofdS8qYLZJzlRyN0FSShK3B2B6CBAE1NzYnbU1auXDVt2vT0jKynz16UlVW8eVNbXV2DZ18jq9gA9+4XrPLxozV2Wv3hOE6r1cXEbuVFtka6qTo6Omtq3t66nXcwO2fT5rjkHbsiIqPTM7Ju3roLx8TSCQpdJZZ0BQ5GIJmy8+aNZeLwTJ+zv6ppJpubW8aPn/iisHjjppjgtetwArI+YsPhI8f1esPMmW5w7o8gJQDEzFo1XRZ6zs7EZYBGrPgIJoHBZyYwHZ1BMTG3yulFYfGY774fP37isCFDRwwb8fxFkVarS9ye0rdX7+MnzlS+qjp7LnfjppiFCxd7r/ItePgYt844hIBhZrBEmJD01URMQSzmKVc9PB0CjEpwGZGzVp2IFLQTCgXFQuIoslZICCGwJBwTu3Xs2B9GDBsxfvzEoYOHDBk0eNPm2Hf/r73r/Kvi6P7+JzEiBo3lYwkYO0FEmgVBBHsDQRTEgthQiIhKVAQiqMTeY4ldrKioWBGVIipNeocLF7g7s78X87snZ2d2l6uS58mLZ17cz97ZKeecOec7Z+p+LmPnhhh8MLmHLFt++sx5aAPsobDfkpLSdesjZGFemRBSWVn9/v2HlD8Oz5gxy8vLO2534qXL1/Ly8tk4i1NoqlzsYGTjkQ5OiWvh2OQexFediq5TqWoVDixIkvT8xSt394n19Q3WPazS7qczZcjJfW/1Xfe8vHxCyLbtOwICgzBTGM05GkRm9U2de6sqN2LeZoZfgb1hmONuXNKvWl9uma/fxCckVVRURWyMjE9IkiSpurrWycl5qN3Qbdt3jBo52td3xm874uDzuF9ahX7AXFMzWOO9dhx3RHlHMh5vshgGNGzam92qA5FdSDYL3US5A5Wc3neV1LiKuEgxMRYruzj6XXbunqT9A/r1t+5h1ecHm7lz5wcELHZ3n+jjMz0yanPWm3dv3rxrbjY8f/HK1dXd4ZexwSGh+R8+4a4Aim1oaJw+fSbzG99l5965m7Y/5dC27TvWrF3PdkNc+OsK+3IL18AizRxfnJ3o8GW5xHQiuRp1StZ5BUC8ddtvkVHRp8+c9/b2aW1tZXo5f/7CkGXL2S7Y11lvx4yxr6qq4dikAjTgAZRILUcqPAMlImuyuScX2cfdNS4KE6DfLvri2hwd8yozy2T6/+uvJElK+ePw4SMn1q2PGD/e5cHDRzU1tfpHn7/CiIBakQuIhK13VBgbMuzgFAPQx2S+WA9/ePOfmgzWamxVhrsqcJ4z9yubO9jS0rLcvPysN++OHjsVEBjk4eHp6Tk1dPnKmK2xBw4ePXrs1</t>
+        </is>
+      </c>
       <c r="I24" s="3" t="n">
         <v>1</v>
       </c>
@@ -2404,7 +2511,11 @@
           <t>Which one of the following sets of teeth is not deciduous?</t>
         </is>
       </c>
-      <c r="H25" s="3" t="inlineStr"/>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following sets of teeth isnot deciduous?</t>
+        </is>
+      </c>
       <c r="I25" s="3" t="n">
         <v>1</v>
       </c>
@@ -2481,7 +2592,11 @@
           <t>Which one of the following maintenance practices of tools can be carried out on all types of tools?</t>
         </is>
       </c>
-      <c r="H26" s="3" t="inlineStr"/>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following maintenancepractices of tools can be carried out on alltypes of tools?</t>
+        </is>
+      </c>
       <c r="I26" s="3" t="n">
         <v>1</v>
       </c>
@@ -2558,7 +2673,11 @@
           <t>Which one of the following materials does not float on water?</t>
         </is>
       </c>
-      <c r="H27" s="3" t="inlineStr"/>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following materials doesnot float on water?</t>
+        </is>
+      </c>
       <c r="I27" s="3" t="n">
         <v>1</v>
       </c>
@@ -2635,7 +2754,12 @@
           <t>The diagram below shows a tin that was used to investigate pressure in liquids.</t>
         </is>
       </c>
-      <c r="H28" s="6" t="inlineStr"/>
+      <c r="H28" s="6" t="inlineStr">
+        <is>
+          <t>The diagram below shows a tin that was usedto investigate pressure in liquids.
+If the tin was filled with water, which holethrew water furthest?</t>
+        </is>
+      </c>
       <c r="I28" s="3" t="n">
         <v>1</v>
       </c>
@@ -2712,7 +2836,11 @@
           <t>Which one of the following is not a characteristic of animals?</t>
         </is>
       </c>
-      <c r="H29" s="3" t="inlineStr"/>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not acharacteristic of animals?</t>
+        </is>
+      </c>
       <c r="I29" s="3" t="n">
         <v>1</v>
       </c>
@@ -2789,7 +2917,11 @@
           <t>Excess water in a home can be stored in a?</t>
         </is>
       </c>
-      <c r="H30" s="3" t="inlineStr"/>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>Excess water in a home can be stored in a?</t>
+        </is>
+      </c>
       <c r="I30" s="3" t="n">
         <v>1</v>
       </c>
@@ -2866,7 +2998,11 @@
           <t>Which one of the following is not a body building food?</t>
         </is>
       </c>
-      <c r="H31" s="3" t="inlineStr"/>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not a bodybuilding food?</t>
+        </is>
+      </c>
       <c r="I31" s="3" t="n">
         <v>1</v>
       </c>
@@ -2943,7 +3079,11 @@
           <t>Which one of the following is not the main reason why we light a house?</t>
         </is>
       </c>
-      <c r="H32" s="3" t="inlineStr"/>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not the mainreason why we light a house?</t>
+        </is>
+      </c>
       <c r="I32" s="3" t="n">
         <v>1</v>
       </c>
@@ -3020,7 +3160,11 @@
           <t>Which one of the following is not a recreational use of water?</t>
         </is>
       </c>
-      <c r="H33" s="3" t="inlineStr"/>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not arecreational use of water?</t>
+        </is>
+      </c>
       <c r="I33" s="3" t="n">
         <v>1</v>
       </c>
@@ -3097,7 +3241,11 @@
           <t>Which one of the following is not a use of heat?</t>
         </is>
       </c>
-      <c r="H34" s="3" t="inlineStr"/>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not a use ofheat?</t>
+        </is>
+      </c>
       <c r="I34" s="3" t="n">
         <v>1</v>
       </c>
@@ -3174,7 +3322,11 @@
           <t>Which one of the following can not be grouped as a cereal?</t>
         </is>
       </c>
-      <c r="H35" s="3" t="inlineStr"/>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following can not begrouped as a cereal?</t>
+        </is>
+      </c>
       <c r="I35" s="3" t="n">
         <v>1</v>
       </c>
@@ -3251,7 +3403,11 @@
           <t>The diagram below represents a certain type of weed.</t>
         </is>
       </c>
-      <c r="H36" s="3" t="inlineStr"/>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>The diagram below represents a certain type of weed.Which of the following weeds is it?</t>
+        </is>
+      </c>
       <c r="I36" s="3" t="n">
         <v>1</v>
       </c>
@@ -3328,7 +3484,11 @@
           <t>Which one of the following is a protective food?</t>
         </is>
       </c>
-      <c r="H37" s="3" t="inlineStr"/>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is a protective food?</t>
+        </is>
+      </c>
       <c r="I37" s="3" t="n">
         <v>1</v>
       </c>
@@ -3405,7 +3565,11 @@
           <t>Which one of the following is not a beverage crop?</t>
         </is>
       </c>
-      <c r="H38" s="3" t="inlineStr"/>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not a beverage crop?</t>
+        </is>
+      </c>
       <c r="I38" s="3" t="n">
         <v>1</v>
       </c>
@@ -3482,7 +3646,11 @@
           <t>The moving parts of a tool are best maintained by</t>
         </is>
       </c>
-      <c r="H39" s="3" t="inlineStr"/>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>The moving parts of a tool are best maintained by _______</t>
+        </is>
+      </c>
       <c r="I39" s="3" t="n">
         <v>1</v>
       </c>
@@ -3559,7 +3727,11 @@
           <t>The set of teeth that are shed off are all known as the following, except .</t>
         </is>
       </c>
-      <c r="H40" s="3" t="inlineStr"/>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>The set of teeth that are shed off are all  known as the following, except _______</t>
+        </is>
+      </c>
       <c r="I40" s="3" t="n">
         <v>1</v>
       </c>
@@ -3636,7 +3808,11 @@
           <t>Clouds that bring rainfall are known to be</t>
         </is>
       </c>
-      <c r="H41" s="3" t="inlineStr"/>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>Clouds that bring rainfall are known to be _______</t>
+        </is>
+      </c>
       <c r="I41" s="3" t="n">
         <v>1</v>
       </c>
@@ -3713,7 +3889,11 @@
           <t>Which one of the following is not a way of using water at home?</t>
         </is>
       </c>
-      <c r="H42" s="3" t="inlineStr"/>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not a way ofusing water at home?</t>
+        </is>
+      </c>
       <c r="I42" s="3" t="n">
         <v>1</v>
       </c>
@@ -3790,7 +3970,11 @@
           <t>Which one of the following list of foods makes up a balanced diet?</t>
         </is>
       </c>
-      <c r="H43" s="3" t="inlineStr"/>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following list of foods makesup a balanced diet?</t>
+        </is>
+      </c>
       <c r="I43" s="3" t="n">
         <v>1</v>
       </c>
@@ -3867,7 +4051,11 @@
           <t>Which one of the following is not a protective food?</t>
         </is>
       </c>
-      <c r="H44" s="3" t="inlineStr"/>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not a protective food?</t>
+        </is>
+      </c>
       <c r="I44" s="3" t="n">
         <v>1</v>
       </c>
@@ -3944,7 +4132,12 @@
           <t>A pupil set up an experiment to investigate a certain component of soil as shown below.</t>
         </is>
       </c>
-      <c r="H45" s="6" t="inlineStr"/>
+      <c r="H45" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A pupil set up an experiment to investigate acertain component of soil as shown below.Which component of soil was beinginvestigated? Prescence of _______
+</t>
+        </is>
+      </c>
       <c r="I45" s="3" t="n">
         <v>1</v>
       </c>
@@ -4021,7 +4214,11 @@
           <t>Which ones of the following are fibre crops?</t>
         </is>
       </c>
-      <c r="H46" s="3" t="inlineStr"/>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>Which ones of the following are fibre crops?</t>
+        </is>
+      </c>
       <c r="I46" s="3" t="n">
         <v>1</v>
       </c>
@@ -4098,7 +4295,22 @@
           <t>Which tool is not matched with its correct use?</t>
         </is>
       </c>
-      <c r="H47" s="6" t="inlineStr"/>
+      <c r="H47" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which tool is not matched with its correct use?
+Tool
+Use
+A. Hammer
+Driving nails into wood
+B. Spade
+Digging
+C. Axe
+Spliting Wood
+D. Wheelbarrow
+Carrying light loads
+</t>
+        </is>
+      </c>
       <c r="I47" s="3" t="n">
         <v>1</v>
       </c>
@@ -4175,7 +4387,11 @@
           <t>The provision of water to plants during dry periods is known as</t>
         </is>
       </c>
-      <c r="H48" s="3" t="inlineStr"/>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>The provision of water to plants during dry periods is known as _______</t>
+        </is>
+      </c>
       <c r="I48" s="3" t="n">
         <v>1</v>
       </c>
@@ -4252,7 +4468,11 @@
           <t>Which one of the following is not an animal that we keep at home?</t>
         </is>
       </c>
-      <c r="H49" s="3" t="inlineStr"/>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not an animalthat we keep at home?</t>
+        </is>
+      </c>
       <c r="I49" s="3" t="n">
         <v>1</v>
       </c>
@@ -4329,7 +4549,11 @@
           <t>The bubbles we see from soil in a container when water is added to it is a sign of the presence of in the soil.</t>
         </is>
       </c>
-      <c r="H50" s="3" t="inlineStr"/>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>The bubbles we see from soil in a container when water is added to it is a sign  ______ of in the soil.</t>
+        </is>
+      </c>
       <c r="I50" s="3" t="n">
         <v>1</v>
       </c>
@@ -4406,7 +4630,11 @@
           <t>Digestion of food does not occur in the</t>
         </is>
       </c>
-      <c r="H51" s="3" t="inlineStr"/>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>Digestion of food does not occur in the</t>
+        </is>
+      </c>
       <c r="I51" s="3" t="n">
         <v>1</v>
       </c>
@@ -4483,7 +4711,11 @@
           <t>The air we breathe gets into the blood stream at the</t>
         </is>
       </c>
-      <c r="H52" s="3" t="inlineStr"/>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>The air we breathe gets into the blood stream at the</t>
+        </is>
+      </c>
       <c r="I52" s="3" t="n">
         <v>1</v>
       </c>
@@ -4560,7 +4792,11 @@
           <t>Sinking and floating is affected by all the following except</t>
         </is>
       </c>
-      <c r="H53" s="3" t="inlineStr"/>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>Sinking and floating is affected by all thefollowing except</t>
+        </is>
+      </c>
       <c r="I53" s="3" t="n">
         <v>1</v>
       </c>
@@ -4637,7 +4873,11 @@
           <t>The diagram below shows an experiment done by some standard 4 pupils.</t>
         </is>
       </c>
-      <c r="H54" s="3" t="inlineStr"/>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>The diagram below shows an experimentdone by some standard 4 pupils.Which one of the following observations wasmade if the tin was filled with water?</t>
+        </is>
+      </c>
       <c r="I54" s="3" t="n">
         <v>1</v>
       </c>
@@ -4714,7 +4954,11 @@
           <t>Which one of the following is an oil crop?</t>
         </is>
       </c>
-      <c r="H55" s="3" t="inlineStr"/>
+      <c r="H55" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is an oil crop?</t>
+        </is>
+      </c>
       <c r="I55" s="3" t="n">
         <v>1</v>
       </c>
@@ -4791,7 +5035,11 @@
           <t>The diagram below represents a breathing system.</t>
         </is>
       </c>
-      <c r="H56" s="3" t="inlineStr"/>
+      <c r="H56" s="3" t="inlineStr">
+        <is>
+          <t>The diagram below represents a breathingsystem.The exchange of gases takes place at the partmarked.</t>
+        </is>
+      </c>
       <c r="I56" s="3" t="n">
         <v>1</v>
       </c>
@@ -4868,7 +5116,11 @@
           <t>Which one of the following food is digested right from the mouth?</t>
         </is>
       </c>
-      <c r="H57" s="3" t="inlineStr"/>
+      <c r="H57" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following food is digestedright from the mouth?</t>
+        </is>
+      </c>
       <c r="I57" s="3" t="n">
         <v>1</v>
       </c>
@@ -4945,7 +5197,11 @@
           <t>Which one of the following is not part of the breathing system?</t>
         </is>
       </c>
-      <c r="H58" s="3" t="inlineStr"/>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not part of thebreathing system?</t>
+        </is>
+      </c>
       <c r="I58" s="3" t="n">
         <v>1</v>
       </c>
@@ -5022,7 +5278,11 @@
           <t>The diagram below shows the digestive system.</t>
         </is>
       </c>
-      <c r="H59" s="3" t="inlineStr"/>
+      <c r="H59" s="3" t="inlineStr">
+        <is>
+          <t>The diagram below shows the digestive system.Which one of the parts labeled W, X, Y and Zis correctly named?</t>
+        </is>
+      </c>
       <c r="I59" s="3" t="n">
         <v>1</v>
       </c>
@@ -5099,7 +5359,11 @@
           <t>The diagram below shows an experiment that was set up to investigate transpiration in plants.</t>
         </is>
       </c>
-      <c r="H60" s="3" t="inlineStr"/>
+      <c r="H60" s="3" t="inlineStr">
+        <is>
+          <t>The diagram below shows an experimentthat was set up to investigate transpirationin plants.Which parameter should be checked beforeand after the experiment?</t>
+        </is>
+      </c>
       <c r="I60" s="3" t="n">
         <v>1</v>
       </c>
@@ -5176,7 +5440,11 @@
           <t>Which one of the following weeds can also be used as a vegetable?</t>
         </is>
       </c>
-      <c r="H61" s="3" t="inlineStr"/>
+      <c r="H61" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following weeds can also beused as a vegetable?</t>
+        </is>
+      </c>
       <c r="I61" s="3" t="n">
         <v>1</v>
       </c>
@@ -5253,7 +5521,11 @@
           <t>Gastric juice is produced in the _______.</t>
         </is>
       </c>
-      <c r="H62" s="3" t="inlineStr"/>
+      <c r="H62" s="3" t="inlineStr">
+        <is>
+          <t>Gastric juice is produced in the _______.</t>
+        </is>
+      </c>
       <c r="I62" s="3" t="n">
         <v>1</v>
       </c>
@@ -5330,7 +5602,11 @@
           <t>The following  diagrams of are different types of teeth.</t>
         </is>
       </c>
-      <c r="H63" s="3" t="inlineStr"/>
+      <c r="H63" s="3" t="inlineStr">
+        <is>
+          <t>The following diagrams are of different typesof teeth.Which diagram shows the type of tooth usedfor tearing?</t>
+        </is>
+      </c>
       <c r="I63" s="3" t="n">
         <v>1</v>
       </c>
@@ -5407,7 +5683,11 @@
           <t>Which one of the following is the third stage of HIV and AIDS?</t>
         </is>
       </c>
-      <c r="H64" s="3" t="inlineStr"/>
+      <c r="H64" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is the third stageof HIV and AIDS?</t>
+        </is>
+      </c>
       <c r="I64" s="3" t="n">
         <v>1</v>
       </c>
@@ -5484,7 +5764,11 @@
           <t>Which one of the following is not part of deciduous teeth?</t>
         </is>
       </c>
-      <c r="H65" s="3" t="inlineStr"/>
+      <c r="H65" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not part ofdeciduous teeth?</t>
+        </is>
+      </c>
       <c r="I65" s="3" t="n">
         <v>1</v>
       </c>
@@ -5561,7 +5845,11 @@
           <t>Absorption of digested food takes place in the _______.</t>
         </is>
       </c>
-      <c r="H66" s="3" t="inlineStr"/>
+      <c r="H66" s="3" t="inlineStr">
+        <is>
+          <t>Absorption of digested food takes place in the_______.</t>
+        </is>
+      </c>
       <c r="I66" s="3" t="n">
         <v>1</v>
       </c>
@@ -5638,7 +5926,11 @@
           <t>Clouds that bring rainfall are known for their _______.</t>
         </is>
       </c>
-      <c r="H67" s="3" t="inlineStr"/>
+      <c r="H67" s="3" t="inlineStr">
+        <is>
+          <t>Clouds that bring rainfall are known for their_______.</t>
+        </is>
+      </c>
       <c r="I67" s="3" t="n">
         <v>1</v>
       </c>
@@ -5715,7 +6007,11 @@
           <t>Gaseous exchange takes place in the  _______.</t>
         </is>
       </c>
-      <c r="H68" s="3" t="inlineStr"/>
+      <c r="H68" s="3" t="inlineStr">
+        <is>
+          <t>Gaseous exchange takes place in the _______.</t>
+        </is>
+      </c>
       <c r="I68" s="3" t="n">
         <v>1</v>
       </c>
@@ -5792,7 +6088,11 @@
           <t>Which one of the following statements is true about what happens during breathing in?</t>
         </is>
       </c>
-      <c r="H69" s="3" t="inlineStr"/>
+      <c r="H69" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following statements is trueabout what happens during breathing in?</t>
+        </is>
+      </c>
       <c r="I69" s="3" t="n">
         <v>1</v>
       </c>
@@ -5869,7 +6169,11 @@
           <t>Which one of the following should be done to maintain all the tools?</t>
         </is>
       </c>
-      <c r="H70" s="3" t="inlineStr"/>
+      <c r="H70" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following should be done to maintain all the tools?</t>
+        </is>
+      </c>
       <c r="I70" s="3" t="n">
         <v>1</v>
       </c>
@@ -5946,7 +6250,11 @@
           <t>Undigested food is stored in the _______.</t>
         </is>
       </c>
-      <c r="H71" s="3" t="inlineStr"/>
+      <c r="H71" s="3" t="inlineStr">
+        <is>
+          <t>Undigested food is stored in the _______.</t>
+        </is>
+      </c>
       <c r="I71" s="3" t="n">
         <v>1</v>
       </c>
@@ -6023,7 +6331,11 @@
           <t>Which one of the following diagrams shows calm weather?</t>
         </is>
       </c>
-      <c r="H72" s="3" t="inlineStr"/>
+      <c r="H72" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following diagrams shows calm weather?&lt;img src="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAZAAAAEsCAIAAABi1XKVAAAgAElEQVR4nOy951JrW5Ym2m+TT1D1BBVR/zq6b/3quBnd1REVFbdMdlZVZ1bak+fkPmd7g9l4K0A4CSSMEEggCYEEskjIO+QQ8t6bZe6PsTVzsmQQbNjmHEYoCCEtzTXXNN8cfvwX+pEe6ZEe6Suh//K5O/BIj/RIj9QrPQLWIz3SI3019AhYj/RIj/TV0CNgPdIjPdJXQ4+A9UiP9EhfDd0MWMT9EUmSVJNIkiRJkiCIRqNBEARFUZ/gafGHqlZrlUq1Wq11eRV7o9JdqbWpQqGYzxfgVSwWK5VKrVZHA1ivN/BXrVZvfXV/IsarbQutrcFA1esNkiQ/5TR9FqLuicgmoelrYATbAd8RQG27catukxgx7luvN2A2K5Vqo9H4yPHBb1Sr1SuVSqVSuVubvdMjh/VIXygFlYG5v5lFr/G/GuX/b15QGfg0d78v2GJAGH5442j1kf0kr9PHN3u3bnyCO/bEYTXuldpyBwj4K5UKvMHPf8QRNK9BV95A5Q4EdwGuAZ14+EoCYnA0jNe9jANjNKBZ/EzuxEx1YpquD1HHV/eLYfAbTUYA32/QGfj5gy5N965r8Gf9rS/zqvlB78ug3sGoFS8YG7jHy3onHAEZckzvT4eknE7UfemivQC3vtuD9E6fmsNqO8G4eIjgo/XbLiN444B2Gt9PeQrdL/W4ke6833q59YM+IADW3N/MZoNZeAl/uTP4s/7xvxqt5qoPeuu21MvQ9TKGjF/hQNN7T0iSbDQ+nBz4OdfL9PX4XL0/7KfcR48i4SN9oYQAC31SzVWByfpkgiGDuu/h3nkcCmNXgWOFNzdue6rJENVq9UqlWi6XS6VSpVJBGsav+gzuhb5cwPp41L8VtWWGP/cYdKRbnYofT50G7UGfsRWwaJqe+5vZzwhYdLuRb10/vaAGoFVTKgeq3rjkCIKoVmvlcrlYLObzhVwun8vlwTgDgHXjfb92uiNgsf5ubuSvhwupUi8X33Zj9Cj3fSThiqFO+qB7gcLbEv74N8q2vdgNu7y6t3OjUuxui6dHagWsbDALHFY2mH3QW3en+wIssKzhetXGTZa7RqNRLpcLhWIul89ksul0JpPJ5vOFcrlcq9U73Rf1k7iu7L/tkyK68YcPR3cBLLvEDetG9v7ofnuDL4K22sT7xYW2oIDv596h9s7UdgRa98Cnp0ZnfT963e/sM4ihwwoqAyv/z9Lgz/qFv9x50Pv2SPhaZRwzRA9uOhRFEU0LBpwcRA8cPRIGK5VKqVQqFIqFQrFUKlUqVXB/IVvY3tZO9g5YXyDdBbAW/34ZAGvybyfvvUM4PfSw3hZNflJ0B7S9X2prJQT8etD73ooQHDAAqxcmi6bpVuwAIIMGW+9FNnXtoGVHXDCOemSLtyODvuq1fWvAiruTsHRG/np48Gf9ZzzTQ3TrkR4JARZyxUKwpXyj+Ny9+wvB/sc5094Bi3ENjlMEQfh8AZ3eEAhc0jTdaDSKxSJBELVavVgslstl3AMGqTgQZjGYdBytHmIQPhndGrBEzw4Gf9a/+PfLW7/fGfxZP+vv5h6iW4/0SG2thO5dFyDXJ/bG6k5UixLjzoxMLJbQ6w0cLr9/YHjw/ShrbpHH31YoTyORKE3TAFJwJUP6I0kSFI64ahIR3qt7eeTPRb0CFox+PlkExkq/fh5zJeC482qDN8oOrRzpo/z1SN2prZWQpmnzqrnt55+XWjma1sXfusgbjWuuDFrd2QJ7ZZbFFu9L3e4LUKgfHStHx6Y4XP6Z4TwajQNOAcPFaA0cHRiu17jj4Y8As24GLBxrTmbVoLrKJQokSbL/fmnwZ/3cX6y1VWl3p06i9RcFYTcCMfVxThU3Nv65B+BzUnfAGv+r0c/RqY5EYYptfHJJkkTyGkMtValUk8kUvCdJ0u2+eD809n5obHdv32S2xmIJQJ/Lyyut7oy7tjH4fvRd3/vllTXlicrj8RYKRUYHCIKoVKoQo1oqlcrlMs5w3UpW/WLpdsHPrL9jDf6sf+/ZPvyrXz8HJivijDPw6Eavgu749YVs2hth937pDrj2GQfnoanV0z0bzJpXzeN/NTr4s37pNwc0TQeVAeEvd74ENTyCJ+I6YBEf3BeqrV4L6XTG7b4wnpvVGt2x4kS8L51lsXeEYpfLUyp9cBgim3JfOp0xm637B7Kp6bl3fe/Hxqc3Nnfc7gv4FuKoKIqq1eqFQjGbzYF/VrlcZrjCEw+ZaOATLMhbAJb14IMS9EIbjDjj8AIJEUEYcRv/qS7b9QvZkA8OUZ1H4Ea0+rwj8wmoUywhoBhE5wB4fTmODp0Bq1IulxH65PMFu8N1IDlc523pz4wIniiKKhaLqVQaQVu9fg3jCIJIJlMXFz61Rrct2JtlsccnZrS6M/gWQCqfL6TTmWw2Vyi0AawH5bC+LMDi/mKt0wIa+ethfOPdAbC+QLSir4vDiOH/jDj1ucfjkxIjWwNK2KCb0KJrdBPaub+Z/YyO7zjhgIWmDAcs/OJ6vSGVHQ0MDq+tb7rdF4BQkHQIXUOSJJ6wBRZApVJNpdLwiezw+Ienz3f39huNRqVSjUSi4PueSKTS6QwCLDzCn3zI+IQvCLCyiTzyvWK84POTWTVjH37VvBVQJxnt4egnDlJfLzFEQjRxJEnW6w0QCYmmDuvqKnx0rJQdHmu0+kDgshOI1Gp1cGFnLAOUJ+NUpRl8P6pQnsK/oLfKZLKRSCweT2azuVKpxJAHf/yABSR7fwRohe8l2GN7z/bBv+Fxsz3ST42oluBnBiJQFNUErCpJkrVaPZFIKU9U7MVVDpcvP1L6fAG6KQyCyrwZHlhtNBrQLAp1RuBFNp0YMpmsTm9Y5fBmWezFJY7X6ycw1T5FUdVqrXHdFomOxk81SPdJvQIWcFIns+pWVEK+DrYDF0VRtgPX2i/WY67Eg/b7kR7pi6VOp3W1WpMfKcfGpxfYK+J9qezw+ORU7fF4wSMUflKvN8A4iPK7Uk1TI447JElWKpVwOOLxeIHhikSissNjkVjidl/goMnoCXk9QOfhBuGBqCfAOuOZWtkrnJA3KUVRAF5rv1h/6K4/0iN9RuoiQwDEML4tl8sL7JWlZe6Z4dxmc9gdLrf7wucLpFJpXLNOEASoyYmbzHkkSZbL5Ww2B5fl8wW73cnjb5nNVnTH1o6Bi8PXi1k9Adbi3y9P/u2kdFDeCbBirsTIXw+P/PVwzJWQDson/3bSLnE/dNcf6ZE+C+H6kE4XkM2gPwCgcDhyZjjvHxg+lH8IKorFEq3R4xSW//NWUAJuDaVSaUco5m8I1BqdzeYIhcK4eEgQBAinKJcsDltfC3LdIjSnE1q1pYfr8SM90mchHKfQbm9d6jiKVSpVt/tCoTxVqbVms9XnCyBmqu0eodqp7XvsG0EQ5XLZeG7mcPmTUyzW3OLWttBisZVKJRynqKYKjGH16vF2n32z3y405xGqHumnSQhKWu3d+G4HBTn6t1AoqjW6BfbK0PD45BQrEom1NguQgT5BgNW9Mzh6olsXCkXwbCgUivsHsnd97zc2d3y+QCQSi0Ri+XyhgXmuQgu3Aix008+4/XsCrEeoeqSfDrVd2witOiUIgwTHAFjA7Gi0+qVl7p7oAKSzbDbXaMnPh1Is4Pr1GwGLbIb7QG4ZhHegiacoqtFoqNTaiclZDpd/KFew5hZfv+k7kBy21g0Br4seJVCqayDalwJYjzj1SD8F6r7IGWjVUqaoAvlXwXGhVCpFo/GjY+XyyprN5oD2a7V6OBzJ5fLwL3JWAMdOgAx883fpKqAM5EoG11AEcPgPoc+pVJrH337y/bNtwW6pVMIBDjXF8HvoMkTdfAg7K/Xuke4IWA/drUd6pAei7uu5LW9FYvn5UBZWcK0CxRDOIgEilEol8b70Xd/gtmAvkfgQ4QxSJLoRgA7DINjaK9wRAUcEgLzWmGqcCILI5wvxeNLr9e+JDmZmFzweL+OaVpTBH7x1KB4B65Ee6RNRJwaqy2VkS2ZhZG4Dbym8EYAhaORYcfLi5ZuR0UmRWOLxeNHnSOLrIv0x7l6vNyAnMiO0kG6yVFQ7Rwr880ajEQyG1Brd4hLnzHAO33bi5ggsd3PbGmJdwOuWE3JrugtgPXSfHumRHoh6BCz8egRY+OdIKMOz5TE2bSqVNhhNEqmcvyGYZbEnp1g2m6NQKGYyWdCLQ9bQHnveaDRyuTzCR0ZnIFwRJXdHQitgDUmS+XxhT3Tw9t2A3e6s1er5fAGyRzD8UdG9qtUaVo/4AyNJXvdHZdAjYD3SI90zMbiDXpY0+gn+SQOrXcLYyXi4MgBHNpvTaPUrq+tr65t2uxMwolAogj2xUqnm8wWGOrxWq6dS6WAwZHe4FMrTbcHe/oFMrdFZLLZsNkfTdL3eSCRSmUy2Uqngd8ffV6u1SCRmMluXlrkvX71dXlmz2hxd6nWTTX96JAWjxDit8T10B8zqMpL3Qo+A9Ug/IWqVZe6wpCmKQjgFrE21WqOagTVXV2FwMa9Uqj5fQK83SGVytUZ3brLMLywvLXNlh8fbgt2lZS6PvyWRyo1GUzAYYmTjKxaLHo/3VKXZEYp39/bF+9J13tYCe0UklhwdKw/lilOVxnhuvrjwJZOp63D5oXxOoVCMRGKxWOLqKiwSS6am585NFnRZq72SJMlyuZzPFyqVKoWpz9ADtmrKvlDAIlvcLh66T4/0SA9ErTqXj1zSlUrF5wuYzdZzk8Xr9Wu0+o3NnaVlLmtucXKKNT4xM7+wzOHy5+aXRsemWHOLL1+9/c1vfz88MiGVHVltjlAoHIlEI5EYiHuo2Xq9kU5nAoFLh9NtszkcTnc0Gi8UiodyxQJ7ZYG9srUtPFacSGVH24K9ldV1CE602hzRaNxqcxzKFecmSyQSBTlRsCN6+uzlgeQQOgwGTeDyoLhhsVhEVV3xp6MoqgtgoWu+aMB66A490iM9HN07YCWTKcilx+Hy90QHsyz26zd9M7MLUpnc4/G2Bt/YHa6NzZ2R0cmBwRH9mRE+LBaLoNLqXvwZcjlEIlG7w6U8Ue2JDuRHSv2ZUa3RyY+UIrFka1u4uMQZG59+PzQ2NT23tMydmV0YGh5/1zf4+k0/BF3PzC70Dwy/63u/uSW0250ul8fpdCcSKaqpvId7UU2fUlBm4Z4TrfQIWI/0SA9CCKduFUbXeg1wQD5fQKs7E4klB5JDvd7gcnl2hOKR0Un+hsBqcySTKXz/IymsWq0ZjaatbaHBaCqXy8jmCCllugAW+nmhUISWS6VSKBQGcTKZTNlsDr3e4PMFKpVqvd4oFIoWq112eOz3B+ECvd6gUJ7KDo/F+9LllbXRsanJKdb8wvLY+PTA4MjiEkcqk2u0eq/XD8YEyDsIunzQ93cfok+AD4+A9Ug/IcLRqseQFKqZ4QBvJJfLm81WkVjC429tbO6cGc6RMAUAxDD/weaH95VKNRKJuVwekPXASwtCl+FXFJanFNWS6I4XOGsDXFgmk0Xqc9z/C0yE8Xjy5FS9yuEpT1SRSDQUCjucbrPZqtHqefxt/oYA8v8lkyk81TLDvNA6UI+A9UiPdJ90B8CC7MMIbtD1V1dh5Ylqd29/d2/f7nDdamuA30CpVMrnC8ViEensgRBaQYJ2yBrae+MEQUDyP/xDBDQkSRaLReRwT9N0NptLpzPpdCYajYNdUqXWSqTyU5XGanNcXYXBPx45cNzIAz4oPQLWI/2E6LaABewViEXIlQG+ajQaoEuSHR57PF7wdYK93YkTIQgC6bzxW+TzBfwTgEiAM3CYYrSG+g/unXA7UCGBaAllvpAHQ73eiMeThUKRJElws0inM12eOhgMTU6xllfWTk7VXq+/XC6jsKQbeb2HpttVfkaqNcbEM1JVMJxcuoBd6zW4Aq9LU1QHX1sUQoF7yqAXI2C1JSKM+YKvkL8vXt/tVnNGYsXp8NsxKpo8ngdfGsEOR+pwUAzBNOn1huGRiddv+oZHJpQnKiTBgcYHYAuU1oVCsVAogiBmtTkOJIeHcoVObzg3WVwuTz5fgKULKIN7aeLrgbGDYEXBJ7Dg4XpGtXr8WZqsYhWWHwBiNpsDZy50GUEQoVDYeG7e2hZOTc/x+Fs6vaE1zwRjlBDd18h3oluXqu+OWd1RplNrd6O2gNW2V13qX3SCtraVvvFnvBW4UFhIGrojo+U7NPtID0cwR+jfer0RDkfc7guj0XQoV/D4WyOjk0+fvXz56u34xIzs8DgWS4BLJ1AikVJrdGvrm3uiA41Wf26y6M+Mg+9HNzZ3QqGwxWoX70vhNcti9/UPHcoVlUo1Fksw6jl3kr/i8aTb40VRijRNkySJ+2Qx1lLb1YXO0Ua7koXxeFKhVE3PzL9+0y+RyoFfayuc4lu+h6H9KLo1YNEdMIsBGW0hplNTD4FZrRDWqXttMe5GFP74cWM0+AhYn5LaTiLZ1E8joQw+r1SqWt3Z5BRrZnZhbX1ToTw1npvZi6vffvdkanoOpEKF8jQcjoAmnru2wV5cXVvfhNKB7/reT0zObm0Lo9F4tVrLZLIAQ/l8wel0K09U24Ld8YmZwfejkUiUpulUKg25q2BJoO4hSRP+VipVjVa/tr7JXdvYEx2cqjROpxsBHK7mJ0kSPK26D0ij0cDxqFwuB4OhbcHu4PvRQ7kCYo9QdUW0Vm/c4/dLdwes7njRFl86tfNA1NrVtt3ovTOdfniHMWwlNHT30tojdSEKS1yHPiSb9biaFv0qkuP0Z8ZVDo+9uGqx2uFiqPqHfm63O1+9fjcwOALO6Dq94eLChzNcoEVqTbJON11P+RuCV6/fcbh8/ZnR6/XH48lisYgrziFrDQAKRVEej/dAcsjh8jlc/uaWULgrnpxivXz1VnZ4rNWdyQ6P7Q4XDripVPpGzT1BECAwFotFlMFZf2ZkL64qT1T5fAEUGjBuuOx54x65R7oLYNFdMavHDd8r6tySOvWW0b27PTWDyCZH3QVlyJ6LlJB3zY3bOhddWrhxrH70RGKp+HAhiPjgJHnNEyoSiWl1Z+u8Lfbiql5viESi1HUHS5qmc7m8w+kW70vB43xldf3kVB0OR3CAIAgCr5CKU61WB/aHIAi1Rmc0mlKpdKlUguBkmFZgjkiSBDVZKpU+kByOjE7iuieH0y3cFR8rTja3hOMTM2/fDQwNj4+MTmYy2d5PQdDTlUolHG1TqbTx3HwoV1xeXuGPg3wdPuWiuiNg0e0w61Zocnssupm6dJUBqXd+apxAcADfv07XwDZAlqNO/aSw6gM99hAffIaqrksjFJZ+AFecdb/jbQf8iyWyma0FmAWEWVTT9YkRG+z2eDlc/sjo5MbmDnzCmO5YLCE/Ugp3xSKxRK3R+XwB0NB3XxVUM+QFr19frzfODOcXFz74Fy0YUNvD/GYy2VQqfXUV3twSPn32gsZirSmKymSyMCmZTFaj1W8L9v7vr/7TYrV3twm29g34LPi3Wq3ZbI619c2x8Wm73Yn6BhZMSDhBYdJM7ze6G90dsOiHl+luRd37SbZk3f+YB6eb8woGoC53r9cbyMbcHUfuAFg4s4CbIHFenfErxk8YqY463YjqIP7f2MkvjeDZYaCQLY+8np4YV+UcyhWv3/TPzC44nB+qQDHycyYSKavNEY8n0S2gZVTxgXFGUhSFzjlgUloLOzNy8mUy2WAwpNMbaJqWHykXlzgcLn9jc2f/QMZ4Oug2QRCQ/qFWqw8Nj79+07+0zNWfGSORGLoRyofTdogKhSLD30qj1Y9PzKBEWrVaPZfLg8sF7uXQy7r9SPoowKK7YtaNF9wj3djPVsDq5VddGqcoqlKpwrR1aQqb2irCkbatIcDqpXvUdbMjQis8DSbRoaYL0SE9W9s7wgiQHYwSXXr4ZRI8O8prjDNZ6JpKpZpOZ0As4vG3v/3uyTpvi2H4x4eaaGY3xiEAUA95riAXB0hqXCqVisUPwYO4Dw3dZF5wBXkqlbY7XH/85lup7EgkltgdLvA1hVRVdFM1AV0im2lhaJqu1xtGo2lmduHN2/6Xr97Kj5R001EDCXStk0iSZCaTzWSygKqnKs3U9Nz0zDx/Q2CzOWCgICUOcjqjviLAontISfoJ8OiBiOEt1doTCHlPpdKgHy0Wi8FgCLQVFEVBWAPKo9Y22z96xlZJrXG95AHyM8blOPK6qwRc2YVpakWfLmIyo2ONFrrPsf4khBgoBtwwroF9WC6XjUYTj7/F42+pNbpWJRRxvSh867d4ZS266TjKyMLeSuD5ifxL9XoDa26xr3/I4/GCYgsF8eChPGTTdxSwDH4biUT3D2STUyy3xwve7Y1GAxzooSnA0LadUZ6oXr56+/pN/wJ7xWA0wbNgOFtBvmZok34dgEV3DX389DiFQ0CXC7q0QBAEWLX9/qDfH4xEovF4MpVKJ5OpaDQeiyWSyVQmky0Wi3CuXl2Fjedm2eHx0bFSpdYeyhUHkkOd3uDzBRD/RZIkg9XH+0lhZxSOVrD40LGMwsrwR8NHrK0y8c7DiENVWz+1u7X8GYm6Xk6CgVaM4YJZSKczIrFkembebnf6fIHLy6t8vkAQRDabQ4HHBEG0tQAyViD1QXVV7T4pcAomEilYLS6XR7grhkyhjLMK96JCyww8QlFTgcDlk++fLS1zrTYHTdPVai2Xy4PjPkVRwE4icARxNRgMCXZEIrFEo9VfXl4BxDf9Wito3BgL+M4r7VZ0P4DVhT4lVNEtmp22TSHNdFtDL6yqXC4fjyc1Wr1GqzebrU6n2+cLRCLRVCqdSqVxy0uj0YAk/+cmC+hfJVK5Rqu3WO1+fzCbzcF0gqW8R64E5AIIiUDaWZSEpHvdAfQUHzmkVDsdGeN12za/EELIzvicxJKsIxGvWq1ZbY490cGx4gSST8mPlHa7Uyo7WuXwdHpDqVRqlfQ7jTnMJuOmjZa4Pxx09HrD23cDG5s7kUgM7oL4REi5B+wYcEDAf2WzOThOIpGYWqObnpn/9rvvJVI5TdPZbA6tSexQ/FD4J58vmM3WBfbK23cD+wcyhhdrJ+rCpN87/dgAi8bUNCCLdeG9K5VKIpEKhyMQmw7sLuACxKOCKQR4q1QqDWltYXWWSiXQdMChxABHxn5Az1Wt1vL5QjqdSSRS8IpG45AZMpvNVSrVZDIVDIbi8WQul/f5AgajSac36PUG47nZ7nCFQuFcLt8aXIaWC9E0SjJSerdOCqPuS+uCYwBW26imj5mmL43QBm79KhqNQ4YWmqbh8IjFEhwu/0/f/lm4K6Zpul5vpFLp1nXL+ATgr1AoXl5eWaz2o2OlSCyx250EVlgwkUi53Rda3ZlEKheJJbt7+4tLnJnZBeWJCsEH2XRwbWqyqojPomkahFmwCFms9j3RwbZgb2Nzx2531usNu8Ol0epNZis4Llis9sUlzuISZ219E/LMDI9MQKo/mqYZeVC7DN3Hb9se6UsErI+/I/GXdNRVVEmJcRlJkul0xmKxKZSqM8O51+u/ugrH40lIqcFoEN7EYgm1Rsfjb09Nz01MzrLmFtfWNyVSufJEZXe4EolUqVRq238EGbVaPR5PBgKXbo/X7b5we7x2h8tisVmsdo/HG48nLy58Or1hT3SwyuGtrW9ubQvX1jdXVtc3t4Syw2O3+yKTyTKUDoCY8EmtVocaB6jMAcgRjP7AZfF4EvKCFwpFMPe0sgkIsHAcRK+7TM8XSbDwGOwPmspCodjqGXBusiywV2ZZ7LX1TYVS5fMFYrFELpfHh4XBOlUqFXBGVShV8wvLao2uKZd9OIHK5fLa+uYfv/l2gb1itTkkUvkCe0WnN0A7qD+Io0HmWsaqA51GMplSqbXrvC21RpdMpgDCFMrTHaF4/0C2Ldjb3BJqdWc+X+DoWLm4xNk/kDmd7svLq2QyVSh8EAB7H70eh/oj6ccMWKD6QZiFLDvFYvHy8spqcxjPzfozo8FocrsvotF4KpXOZnO4pNOM0qgolKrxiZkF9grUAjg3Wcxmq15v2BbsTs/MsxdX3w+NvXj5ZpbFlsqODEaT2+MFlr5ebySTKZTRMZFIGY2mM8O5yWw1Gk3Gc7PPFwDxMxZLEASRyWQvLnzQuP7MaLHYLi+vEA4WCkWGAzTwkuVy2e8PmsxWt8cbiyVisQQo3cA62QrW+XzB5ws4nG6XywOiLuTJbZXy4DDHRw9/feRMfSEEBg14DyOGvoLcBplM1uXybGzuzLLYE5Ozqxye7PD43GSBKvA+X2CVw3vx8o1UJvd6/Y3rlQeJpl94Npszm63rvK3JKdY6b0urOwuHIwA64LRVqVR5/O25+aUDyWEwGKJpmiCIeDwJjDw+iYiZ6kIg34GfFEiO4ChPEAQUhR6fmOFw+WazlcL0p5FILB5PglK/k0W7lX7SgHUvN2UAFojoUIbE5fKYzFaFUiUSSyRSudlsjUSi4HiCm1eApqbnpqbnWHOL8iPl5eVVNpvDdatwsoHpBz7xev37B7LFJc74xMz0zDyHy5dI5cZzcygURljQ9hnBcAPvUc/xRQlP1MoBgV8yqFHhGS8vr8LhSCQSSyRSID+2Lu50OuNyec5NFovF5nJ5AoHLeDzZWruFxgCrbTaL3mfkSya8bjMI44VC0Wpz7O7tr61vLq+sLbBX5heWF9gr4AN1IDlUa3QisQRyt8+y2OzF1QX2yujY1NIyVyqTO51uUC0Bt5tOZ9zuC+WJanllbVuwZzSaIpEoPpXlcrlQKMbjSf6GwGS2wodg1YF8e8lkCqaG6KF4Kk5wPeRuB1BGUp7bfbG2vjkyOvl+aGz/QBaPJ5EWDFT+aExum5DrQenHCVjIGwXleM3l8rFYwu8POpxu2KXBYOjy8oqhVqxUqtlsLhKJ+f1Bt8e7yuGtcngard7l8kAVgFYdB9WsrIk8AGu1ejKZcjrdiBd79vzV02cvFpc4sO71Z0Z0DsMBWygU77D/KYpClml4zGw2B0vUzZAAACAASURBVHwiyhLJWNk4x3RjchtcG9gOsHqSF74KqlQqFxc+vz8YCoXNZuux4kSt0enPjCur62/fDXDXNi4ufJlMFjTWyJkgny+4PV6d3uB2X6TTGa/Xv7K6/u13T8bGpxXK02g0TtN0JpOFVC3zC8tQUAc/vegPDn0VMN7NzS+dqjTwOc6poevJZhBfL7wPmnrQakEjuHYCVKiBwKXs8Hhpmas8USUSKdDYNq6HMX45Pnc/TsACQj5ykOw1Go2HwxGfL+D3B9ta6+r1RiyWcDrdOr3h5FStUKpAQYA8CVAne7SJVCqVy8sri8XmcLoNRpPs8HidtzXLYi+wV1Y5vMkpVl//0OQUC0JYpTI5Q1FSLpfBf69t43hncKetTrZRWOuQsKmXoWvrkto0J1WQ1+KPg9LpzO7e/smp2u5wicSSWRZbIpUHgyHwYECXUU1vI4IgwP8OOG6KorLZHHixNBoNlVo7Nj49v7AskcrD4QhN04dyxYuXbzRafevUEM2QoEql4vX6I5Fod38Ropn9qvsTwXTjmUJh7tAP8/nC5eVVJBKLRuN6vWGdtzU+MTM0PL4t2A0GQ1+sgvLHDFg0TUPGtUQiFYlEY7FEq8aabgpW+XxBo9Wv87bAR65arTHgo23fgFvpIu1XKlWI/4J/A4FLqUx+qtLYbA6oCGCx2Pz+oFqjW15ZW15Zs9kccCVuYm+l3kETEWhJQOnb/cDEeUZGxsEfK2Dlcvlzk0W8L4VULfozYyBwWS6Xb7sgqWaG0ng8qdboOFw+d21jRyjm8bc3t4SwDDrhEThSdDpv8Ms6hSUwLgPWG/lPwXvgxEGnzvBTv7oKq9Ra1tzi9Mw8uF/B5zif3sutH5R+5IDVaDRyuXw0Gg+FwkgsB0JhDVdX4aursM8XWFzi/PnJD1rdWdum2rrtAAT0nje2UChGIlHgcQgsgj8UCk9Nz/3+D9+8HxoT7Ih29/YFOyLhrvhQrgD9a+utb7t0ALCaXs7dxE+qGWjSIRfrjwSwEH9aLBbBt064K37ztl8ilTPmGo49nCvvPvL1eiORSJ2cqllzi2/fDfzw9PmT758NDI5AyGEkEkMpse7W7V7OKgAs8KEBFQH466TTGTDLMJQh0GCj0VBrdH39Q89fvD45VcNXSLlJUVSjpf7zJ6abAYsRw0F2DtRA1Br2gcCIanr34G7c4MNdLpdB/YnzsYgYwb2dWI9yuRwOR0KhMHgzqTU67tqGQqkCTwKw0J0Zzo3nZpvNgfAC/BUgfRpN0xC1gNqkMJ9vNAiQIA2iKPAjiGoJl8EjctAmYVijEZrY7c5DucJud8ZiCYPRtLklVChVFotNIpXPsthQ8vdAcrgnOtjd298/kMmPlJDQEjToYFLM5wu5XD6bzYFtCBdpiWZRKTTgeIYQpPuD68nrQTxoZtGk3HHRfW4imuX20DGTzeaOjpV7ooMDyaHd7gSLB9EhdyO+Htru3mq15vX6jefmo2Pl5BTr6bOX67ytiwsfSGRoYCuVCnIPpjBhE22iW0ED1czAV8cSgjMOGEZIEBIb8RtlMlngDTe3hPIjpdFoAlEXNibakp9LsdVTEQp8zhjruBNU4ZPdykaR13OcV7Ds6ThOkddjVpCc0gpYwL0TBKE8UQ2PTCwtcxXK05NTtUqthRIg24K9A8nhyalardEplKcL7JV3fYMoXYbH490/kFmsdnBGR1MIu/rGAkedTrxWpGNwkYz3FEWlUmmv1w/KBYfTrdHqDUaT/sw4MTn7q1//RiSW+P3BQOAykUhBoghwp7q48G1s7vQPDO+JDsABFTWLBq1cLmezuUDg0mK1G8/NAHAWi81qc/h8AcgY11zlFTCEQzGVbDbH0Gigmb1x8XyZhPY2rNhKpZJOZyKRmNFo2hbsjYxOvnz1lr8h8PuDePIWtCa7MzhoWCC5aDKZ8vkC8wvLv/3dH5zNlA/oymYO+A9o0mlt3Iqq1VooFIZgDHDKAaCBUwrMjqlUmgE3eEpScKh2Ot2nKs3a+iZ7cdXnC9ytM/dOdylV3wmz2qJVJ8AiWvKptzbCmDOEWYBu5HVXcrfHu38gYy+uzswuHCtO4vFkOByBnQ+qUEAiuD4QuFSeqPgbAp3eANW9j46VTqebsTO7G+9x/qjL8qKa+S1bH6rt0gfgLpVKbo9XfqRcYK+MjU9DZo9twe7+gSyRSKGgQsDuSqXqcLoPJIfbgj21RofiVNPpDCARrN1SqZRIpC4vr3y+QDAYuroKRyKxSCTq9wdtNgekKheJJcoTlVR2tLG5w13bOFVpGLnoGM/+NRISeNGmrVZr8XjS4XQrT1RLy9zRsalDuQLKQ8BCxfMutH12smnTAC/cRrOQF6T0kB8pxydm9g9kqJoDgz8FFhv9S1FUFzGCsQcZ3zYajWw2BxV9jEaTw+mWHynBVfDV63eTUyyT2QqgptWdWax2ny9gMltVau3FhQ/4JkA3ny9wcqpeWuYOj0xsbgntDlcslgCunKGGQ1v+E6yKmwGrlSloxSwGdUerTi0wmLi2s4XORlhAeMdUam3/wPD4xIxILInFEowfwq6GgFWLxSbcFY+NT3/zp+9mWWyd3gCMBliF8F+BxId/whCXUOPdx5BoWtwYnBpjbHGCTLXxeFKhPF1eWVNrdNATgiAQ38e4b7FYBBlkW7Cn0xuAF/P7g8lkCnYaJib8JfSM0Ug6nfF4vPozo1QmF+9LoQ5w28jer5TQEsIHsNFoBIOhUCgcDkdAAJ+YnH356i1wrMBvIgmg7XTX6w1wvEokUpBAGdRGYLiIRKLGc/PyypryRAUeJ3hlQLqZdxT9i4S7ViCgWsIP8HbK5bJILHnztv/1m76x8emV1XXxvlR5otLpDUajCayB74fGXr/pAws1j78tlR3x+NsL7BWF8hTc9yDSI5lMnZss24K9ySnW6zf9b972bwt2vV5/KBTGQ0GoZsK/Hp0tPpI+tgjF3dCqdaO2RbTWW5NYpChknobAAtbc4pPvn/7nb363uMQJBC479bxarUGAXjAYymSyk1Os0bGpbcHu5BTr2fNXrLnFY8XJmeHcbLaazdZzk8VgNIFEptHq9WdGUHIRzQxnqOfwBvQFnQKqb6uYQGio0xtYc4tgCgDFGWAZHucFrH6j0YAgtVAorFCezrLY74fGhobHtwV7DqcbQl6LxWI4HEkkUrFYAqn/ccrnC+FwBAF3pVJheP//CIho535ZKBTBqR0EbbVGt7TMXVziCHZEKHsfRVHA27YuTjhI8vkCOIuijFfoglgsYbM5doTiWRZ7bHx6corF428dK05Uaq1Gq7dYbB6P1+F0t/oGApHX821RmLYLX1F6vWGBvTIzuwBxP/T10xSuBNcNg9EEXlfBYEihVIHS6lCuUChV+weypWXuLIs9v7AsEkvMZqvX6/f7g+cmi/JE5XJ5cA6LaGaC7642uS/6qJzuDMzqEap6aZnBiKFDBudrUqn04hLnj998OzQ8LpXJTWZrMBjqEl8Okjn6N58vHEgOp2fmZ2YXTlWaWCyhUJ7CSlpa5s4vLE/PzO8IxTtC8fLK2vTM/MTk7Dpv6+RU7XS6wS2YpmncrQkKFsTjyVYuncKqHrQdAdgJDF/zy8srlVq7uSWE2gSg44dgC3Bf9vkCRqPJZnOAhYHx7GCRdHu8J6dqkVhisdoB4t0eL/ijAYrRTasWWoUgFLQ+xY+GSCwxC/45zubkcnnliWpicvbZ81eQ5wAIXNjbxl02mqlE4VCBN+gCuJfx3AzJ8E5O1ezF1e9/eP7i5Zux8WlgioHf8fkCaJEgPALdE44U+AaBszCXy09NzymUp3DB1dVfWCF43kqlCq78aM/Ct4lE6lCu4G8Ilpa5ELITDkfwB/T5AtuCXQ6XvyMUezxemqaRyQKeum3I6kPQR+V0xwHrboxV22ZxtGo0Uyk2mvGfaJGdqjSzLPYsi200muATYMUZYwdTVS6XLy58ao1OrzdAHpiNzZ0doRiKi5RKJXAZ1erO1BqdVnemUmsVSpXT6XY63Saz9dxk0erOuGsbA4MjY+PTHC5fdnhsNltdLk8y+RcQLBSK0Wi8rfmMwsyjoOnAvwUFUzKZAsiD6OVzk0UklthsDji7ALBwZqdarUWjcdnh8fzC8tGxEnRb0Whcf2bU6Q36MyMES25uCUdGJ/sHhvsHhgcGh4eGxxfYK5NTrIHBkaHhcdbcokKpahWif8REYuW8GNuMJMlSqRSJxM4M59uC3VkWe2R0cnGJA2uMoihUWR4aad2lCA3BdsH4liAIcIyKx5ObW8Jnz1+trW9eXYXhW7vdubkl5G8I7A4X3hrK4Aj3Rao0YLLwPbW1LTSem+E9gyNDK7B1QGq1ejAYMputBqMpk8nSNJ1KpRmKKjCkQsw2cFWwzr8mwMI5oFa0otsJej02C++BdYftjTYqjHi1WgN/cbvDhTY/SZIQkwXnJLAtqVQagnIO5YqlZa5ILLFYbJDfimwm82ZEERJNE35r92q1ut3u3N3b5/G3wW1dJJbgP7y6CiOei2oRewE6we0efQ7wlMvlgSGy2hyXl1epVFqj1fP4W+cmC7QDjBWjP2iVFItFny8Aaw5sCPwNgUgsUam1+jMj+F6DyBwMhqAPFxc+p9NtsdpFYsnyyhrCfaAGFhrSy8R9XUR28EuoVmt2u1O4K17l8BaXOFvbwgPJ4czsAmtuERgclH6PoigAjrbtN7DE7WhpIfYZ6tBAQA+ELqIL9kQH7/reS2VHlUrF7nDt7u2bzFbQ4gMogEIAFHBg+YWFmk5njEYT1GRF3Wg6uFfbJoOmr4ssqOedVJZnhvOJydn9AxlYseBDAK8e/RA/nj62CEUXtPp4ajKclbbRJLMs9jpvi+GPDuH1aInAaenzBSAH2+ISR6PVg6dSLJZgMGI39geWC9J0Vqu13b39V6/fCXZE3LWNmdmF8YkZ1tyiWqPD4Y9sySoFnxcKxWAwBIs1l8vb7U6j0QSeYsJd8dIy91hxEolE0XrqLqaBSYFugmY8nmSoYymKgpwQYPCu1epo6NQa3es3fSOjkztCscViy+XyraPxac7Pz0IkSYKJUKc3HMoVO0Lx1rbw6FhpsdqDwVAkEtVo9QqlCi5G2S9gcXYaFuIvCY4qaCJwficSiUJIM75Z6vXGucmysbmztr65sbnD3xDw+FusucXxiRkef1unN4RCYbzb8MbpdK+srs+y2EvLXIvVjmI5qKZV/WO0S/V6I5PJnpssu3v767ytjc0dvd6AB0tQzaQUd2v/tnQPVXMeCK3QLcA8jLO+lUolHk+u87ZOVRqYCTTxIDqhOORqtZZIpPz+oN3u1OkNCuWpRCo/lCvc7osuqVTQcYEUBLj/J9HM1Q2CMEEQEEem0xv4GwLQUBiMJnRsghyH9OWALD5fQCqTT03P8TcEZ4Zzm81htTnODOeQhxdOsGQy5fF4Eax00n914vMZa7RWq0ej8Vb3dIRNZrN1cYnD42+fnKp1eoPL5cFPWjhFe5ixr4/C4cix4kR+pBTvS/dEB1LZkV5vwGVkwHd438CymHdZ6uRNNSvJdk4J1WotmUyFQmGfLwCqxlQqHQ5H3O4LyA8hEkuQCoIgCLvduS3Y3RbsHitOUEYaPKsfQitcaqlUqqiME6NL+IfRaNxitZ+bLCAds+YWRWKJy+VJJFK1lmTfvY30PdD9ANZDQBUQ8L2ZTDYajYO0Va83TlWaySmWQnmKjFmoDyBC4kmgQGeUyWTBLpbJZCENSzgcaVx3Z0d8EEPyx/uDFkTrfNM0bTw3Ly5xZlls7toGRAWSJJlOZ5C9BvLPjI5Nffvdk5ev3sKVB5JDl8uDrml6J3/QEcAh2Xbdk02He1h/jGuAt4fA70QiBd5YbVsAjy0YtHQ6Y7U5ZlnsoeFxXD0HjhS9TdpXRiq1dmV1HQ+Bgl0NZhBI0QMKrx4bxPdF9ytxLTDuk4i+BQeIbDYHTen1Bkh3cyA5tFjth3LFOm9LpdaiOmP4uY7WBhzh0B9Qn4GluFQq4UsC5Ec4mFEf7HYnf0MgOzx2e7yg3kJ963E07pfus8zXx7TQ6SvYvWBwSaczao1ufmH51et3T5+91OsN6ErkNADWmdr1Wm+4QgGif6GQUaf7NhoNkBm79A0tNXzmSqWSw+ne3BJOTrGQSghpGarVGmipgGlqNBqRSFS8Lx0dm+Jw+W73BVxPXE9WQzbTRbT2BMkdbd2ygDktFougIOsScws7E//Q7fFuC/aOFSf6M6PT6U4kUr1v16+O7A7X5pbw6FjJELhA+4MbTx/i7tR1P+rWWcY5aLvDZbM53B7vAnvlt7/7wyqHl0ikcO0++jnVLCMAhx+SCcrlMmToZkRE0DQNBi60igxG0/TM/NDw+PTMvEJ5eqtqrA9HnxmwcKGytZ1CoXh1FQbWwOl0C3ZEHC6fvbj6rm/wh6fP9XoDGlyU1AnFiDFuhA4xOLJQoaS2VCgUzWbr7t7+jWw/iHiMzzVa/fTMvK6Jp3COgR0QXQPuyEjuODdZNreETbf1Cp7NBqJqGJhFYTZHZELqYrHqDjcMdT6YvcPhCEoBjHJI/CgpmUzJj5TTM/OQE8bQPGkYg/aggg/aBZ0ugLWNbDXFYvHcZEE5Zhle8kS7TPwoyUwnx2OcsaJpGtLdbG0Lh4bH9w9knQCrk/nigejeAOvOv8V10q0xN7lcHjx3wYXd7fGWy2Wn0w3y/JnhHOmtgWB7w4mEdAQg+MCYwjGCkiYTzSqY6KbVas3j8UJKs14eAbkgghwRCFyOjE7+/Of/8+mzlwqlCvHqZEtxFJqmIR0oQRBWm+PkVA0HbO16bU5IBI5imJEHDRzI9XbFbPBQpzpWnqDTIzSwWseAmBRFFYtFo9HE42/Pstg4M/sjo3y+AOlAFUrVyaka2fVpmga+HreW9iLlfQx1ugXVVJ/n8wWG7jWXy4NfGJp0FG+Lr4Fm1o2/FOlq2wH87tVqLZVKRyIxt8fL429BBWnjuRmY8QZW8wJMkD8JwEKCFWA/uEShJWKzOVZW18fGp6dn5lHqWKBGowEelRqtHsVn0U2NFUjsmUwWTNEgN9WvF+YFGRPC0PGYwVgsoVCq+BuCBfYKMgnDAxIE0TaQCvzOk8nUmeF8c0u4Ldjb3dsfGZ384enzo2Ml3awMznj8Wq2ey+WhbA+ku0TONWSzChOMST5fQJiFQxIjLh9PdYRSX6CcokhFwrAZYeNfARchaAfQHGRwlHLnRyYYVioVvz9oPDfviQ5WVtchODmbzRmNJr8/CKMKNUeRgYXoOdP5HQjkOHSgNhrXzifYIxDuzjBD4+qqyvVy02QzcBKm9caghabcUGHwDRqtnsPlz8wuwE6ErErNVfoXM9dD02cDLBytGn8pc1DBc5lDbQUef+td3yCyKyNye7zg5I04LOS3FQ5HvF4/bDnI4Y+2JS4f4d1G7w1G0wJ7BecpSJLM5wuJRAppnZEVBk1qoVAEmw66RqFUvR8aW1vftNoc8FCQozISiQWDoYsLn9t9AY6pTqfbanO43RfgX4MOq6Ya4kMSG7ygRmv6HciywAAsPAkyTm3PWMTtwkNVKhXjuRnKq1ibNcq/dmI8BTjr0jQdDIZevHzzp2///MPT56/f9E1MzorEEqfTjQwmuCjwoPrmGzcUZLnCWWYCywaOEp+gk4n8kLOhCtFCvUdZgUtQOBxxuTyzLPZ//N9fj4xOGowm4LDQIBAtBa4flD4zYDGMIzDWqLV4PGkyW3n87ckp1qlKgwt6rQrmRjOkvlgsOpzuY8WJzeaAbA2gkqzV6plMFrgqZICDn0PcA7xXa3Rj49OQFOHoWAkvi8UWCoXtDpdObwgELkGhAMpLaJwgCKgtiNDQ7b7YEYrZi6uzLLZgR2S3O+Px5NVV2OF0nxnOT1WaU5VGo9VDZi6T2Wq3OyEhKn5YNQ/PKn5y4qJfA8tRhRAfXczI2EO0BCR0maBIJDrLYvP420ajKRyO/Dh8GtDpCEOKJisajXO4fKjIsLkldDjdrTFeSDf0CXyOIEgIX+TAj0PnURYtoqUIG+K46/W/TDcOWK2ZgtryjOCHrNHquWsbUFxDoTxFHvkMelCuk0FfCmDh3C9cAFxApVKRHykHBkdGRifX1jdVam0wGMrl8m0TnsBsFQpFi8XG3xA8+f7pt989edf3/u27gf6BYQ6Xr9boLFY7uHcbjaZQKAxzj/uVxGIJk9kq3peurK6bzFaT2fry1duV1XW93rDK4T199nJkdJLH315eWZtfWD6QHMIsgsMqLjFBT8AAt7u3r1JrgYuGIH6cQBDuFDWNa9ZbdVVoURJYTkSEVuiFLqawkMzWjQeb4eoqrNHq2YurY+PTao0O5peRcvMrpUazZgf4KyB2HgBLIpVfXPjQlm4dn4cGLIIggJcH589YLGF3uFwuD6pb4XJ5pLKjA8nhqUpjtzsjkRiIEQxCfDSsDaRvQXFF6Hag28KfCIIxaJoOBkOyw2Phrlgklqg1Oo/H20s1gIeme0iR/DGAxVCs4O2gDZxKpY1Gk1R2JNwVS2Vyvd4QCFxCtkaGhQ72YaFQlB8pp6bnPB4vBGdBlYelZS6E5qg1uqNjJY+//c2fvvv3//jVN3/67rs/f/+ubxAVLKFpOpPJuj1e6FsqlQZAgZIqEEHtcnlAVp2cYsG6x1OA1+sNSIEGge8Wq/3GxMRdRgnXYuDgVcfSj5DXy+GgF9LQ4dpWqpk9gnG7ZDJ1eXllNltHx6Z++W//MTU9hzK3gaPWbfv/pRFs3WKxCOWFALNomk6l0sJd8dDw+LPnr/ZEB8VikcKiVhE9tEhYq9Wz2ZzfH9wRil+/6f/jN9/+5re///OTH971vR8ZnYSw/Mkp1vuhsQX2ikQqB+de3HaMLxjESiPjIBS1h/6TJAkWqlZvrEO54rs/fz8xOatQnlqsdr8/CKk+Huipb0W3AyzqOpGd6UYUQww27LG2iwP/FxRJUtnR0PD42Pi0/Ei5u7fvdLph48ViCZFYApHJG5s7kAFj/0AG+YAuLnzgLwf5Nk9VGqnsSLwvVShVA4PD//TP/zo0PK7XG1AoXyQSAy8VMABDHvRcLg+TTTSLHoZCYQ6XPzwyEYlEAR2IplES1PCofG4Vq+QKaiaUhATaj0bjNptDrdEdyhV7ogMef2ttfVOt0V1eXl1eXkUiUSTV1ps1pmrNChFQxAzUE2Qz924ulwcXWdyNKJfLX15eud0XkNIIxKJMJmu3O0ViiXhfenSsVGt0yhMV5HWDOB44lpFCpMf5/SqIoihQCSUSKaghGonENFo9f0Owu7ev1uhgECxWu0arRxw0DD6UC8SZfQKrNw5qHUyir+Jj2Gim94OENvF4Uqs7gwQv67ytxSXO2Pj0zOzCLIsdCoXZi6tXV2Gn090/MHwoV+Ry+fdDY//0z//629/9YWx8+lhxYrc7HU53NBqHoDRcB4okPrTdcLaAJElwy4IHPzdZhLviA8nhuckCMUnRaBxS0HSqyPvp6XMCFokpwlvVwDiiIzgrFouBwOV//MevFtgrFosNogeGhsf/8R//v7fvBlRqbTKZIkkSYn3PTZZoNA5JGsT7UoPRdHUV9nr9RqNJIpWvrW8uLXMh4+i5ycLh8oPB0PDIxL/8yy9sNgcqcFLHcsnjnS+VSoHAJYfLHxgc1p8Z7Q6X2+P1+QJXV+FMJovroWBXwPtIJKY/M5rM1osLH9RbjseT0WgcVgOU+QXJMZPJSmVHA4PDL16+GRoePzpWptMZUHi15rfFCRQZ8D6ZTLlcHuDkY7GE/Ei5tr45M7vQ1z8kEkuCwRCUMrdY7airIFeiZ0SAi2vuGcL7V00gFoF7LcBHMplCVY40Wn3/wDCEK42NTyuUKoCeVCoNhUuCwRCeswinRqOBZ+kjSRJMLpeXV/oz457oYE90IN6XrvO2lpa5ssNjT7NaeKPRMBhN24JdtUYXDIZ+ePp8lcOLRuML7BW3+2KVw9sW7IbDEeWJavD96P/6X/97aHi8f2B4W7Cr1xs6VQYB63kqlXY63RqtHlzkZ1nsldX1bcHeAntlfGJGdngMRxQAMegu8MT/N+o9PwF9fsBCeoEugIUOsUwme2Y4n5tfgrC70bGpf/iHf3z56q38SBkORyDd4pPvnw4MjvD421vbQqnsCGo0nBnOV1bXnz578e13T354+nxgcHiBvaLR6sX7Utbc4oHk0GS26vWG7394PjE526Xb4BWVy+WvrsIejzceT9psjr7+oXd9g+MTMyur6xKp3O2+YKiokUbf7w/u7u1DLvlisRgMhhAWAzKipyZJ0uv1QynDpWUuxIuBXLwnOoCcRH5/UHmigt3l8wWWV9ampudmZhdWVtc3Nnf2RAfyI6VCebq1LZybX+Jw+YIdEWimAKdevHyzvLJmtTmSyVQX9CGxBPwMj4ouA/W1EHXd0bzeLOwOyk10mdls5fG3hbti5YnK7nB5vX4Ol//k+6crq+s+XwD8HhKJ1MWFz2S2Qg5IhB3ImpzN5iAV9cTk7NNnL4W7YsjCNjnFEu9Lr67COLMGKlefLwAJQg1GE2RGGnw/usBeWVrmvnnbD4mzXS7P8xev//0/fiXelyKoJUkSWc8bjcbFhU+hVK2tb46NTw8MDo+NT28Ldo3nZofT7XC6IcmH230Rjyfx3AGoqdbd/cDT0pHuDlhd0KpHkYHCPBu6DASBpbvO5fJS2dH4xMyvfv2b//7f/+6f/vlfIZ+G3x/cP5C963uPEr8CqwypFGdmFyanWJtbQrVGd2Y4NxpNFqsdijmD5Q6O1gX2yu9+9weLxdalz9ls7kByODI6KdwVo0iOaDSuUJ7OLyyDokGl1jI2M1pGbo93Y3NHKjuCIOdQKByJRCG6otMQXV5eqTW6rW3hAnsFvMPeD41Nz8xzuPy5+SV4WJVaa7U5PB4vOElEo3HYIRaLbZXDkx8pvV6/VncGaQA4/NGIZgAAIABJREFUXP7Q8DiHyz8znEO+duK6i3PbbtSwYtHo1eUnXzh1X58EQUDtr1KpBJdVKhVIKzQ3v7QjFBuNJpDf1Rod6BDS6QwK7oNyhAvslQX2ilZ3BrHu4Ny3yuGxF1effP/0F//n31hzixcXvmg07vcHZYfHyytr4MgOQDM5xTo6Vvp8AR5/64/ffCvcFZdKpWPFyavX7wYGR/YPZJeXV1abY/9AxppbnJic/R//4/8ViSXRaBwSovH4WxOTsztCsc3msDtc5yaLQqmSSOUOp7vTxJEkeXUV7hKGhZCd+FQZ3FvpYQHrRiaL6iHZA5h10L+lUulUpekfGP7jN9+i0mmhUDgQuIxEYjhf5vZ41Rqd8dwMCZFNZuvG5s70zPzA4PDrN33PX7z+4zffPvn+2cDg8MrqulQmB8Of8dwMHnG1Wv3iwndx4fP5AqAhksqOXrx88+r1u6npOe7ahkJ5CkDj8wW2BXvjEzNSmTyZTCEtVTNi64NzWalUEu9L374b2BGKk8kUqH5BD9ploBKJlNXmkMqO+BsChVLl9fqh2VgsodMbtraFx4oTl8vj9wfBhwNK1YMQB+Kw2+MFFZ7bfWGx2s8M51Bjgsffkh8pwdvoxqlv6z9946++QMLXcJfLwGWUxDyNE4kUpKCBow7841c5vHd973/3+z/+5re/h2AMq80Bwn4gcAmxyq9ev3vztn9yinWsOMG9XoaGx//lX34h3BWjm+7u7RuNJjD1Pvn+6Z7oIJ3OnKo0Q8Pjao2OpmlIKCg/Ump1ZwrlqXBXLNwVW20OgiD4G4Jtwa5UJl9a5g6+H1WptbVaXaXWAvs/M7sAuUwhDL6TnydkiO40MgzA+iyY9TkBi26RMVulQmSOBYdvOKxmZhd+8X/+bU90IJHK5xeWjxUnkPKCbGfIALxoeidVIEm5x+NVKE9HRiefv3j95m3/4PvR0bGpd33vX71+Nze/JN6XivelYNAViSWCHRFrbnHw/SiHy1coVRubO6y5RfmREoXdeL1+8b50cYmj1Z2BwjWdzrhcHp3e4HC6E4kUQRBHx8q+/qG5+SXliQo8ufAR6DQ+YDaKRKI+X8Bmc/D4W2azFUYG0hyDLgwqteAnJ2ijQHplDDhkChTvS5uZxbcZ5afaElqpuPnpxl99gdRlvdEtwcNEM5NMK0AnEimz2Wqx2t0eL5SYR8cqZImBZMpWm0N2eOz3B+ErsIfgeoBTlWZ+YRmmNZFIQWWtpWXur3/9G5FYQlGUzxcQ70utNgdqFinpQSGAT4TfH7y6CiOdKegucHcEslk4FoxIuCqAbOYybTtoSBjC10CP2/we6UEAq8dDrG3L+Ie1Wh2SYBAEkUymwJi1uMSRyuRWm2Nufkm4Kw6HI3hJNfy34KrrdLqPFSdgd+NvCLa2heu8rYHB4V//+je//OW//8M//OPPf/4/f/7z//mvv/jlLIuNyg2cGc4HBof1eoNebwCTGdKtGo2mBfbKtmDPZnPAykinM3aH6+RUfShXgJvM7t4+a27xXd/7oeHxVQ4vmUypNbqBwZEdoTgWSzDWRNu4ZZqmk8mUxWqXyuQgXyyvrCGfLwTfKM83RVFtja2tBAoXupmA8MXLN3iOSqpD+Y9PvzQfgloPSOp6xAXOPnRH50ajATk/kDkYOY5AfELbiiStw1upVJQnqo3NnXXels8XyGZzFouNvbj6X//rf1tgr9A0TZIkGHPARHOq0kQiUTg7oYQd0v82Gg3QlKOAXHAZZdyR6JqzH9/arR5ejDG522b/GLp/wOp+gnVvmfFhpVK5ugrDiQQKZpFYsiMUn6o0bvcFBN+1baparcViiVUOb2Z2AWXRBCs+aFWhvsOfn/zwr7/45Z+f/LAt2AWjj9XmwFkSWJGM9q02B3dtY5XDE4klXq+fbhrUoPSpVnemUKqUJyqPx5vN5ixW+45QvH8gW1vfXFzitPIyICqC4zLd9JDC/ZXJ69ZSSPccicRaYRp8FPASTK0E5zNN07VaXaPVj41Pf/vdE1RkAQ9k+0oZqO6ELzO0jAnMNRcPZupiEepEYN4FhxUGYCGPByQ0kE1/qHg8KZXJJyZnJVI5FJF3Ot3Pnr+Syo7Qz8GhN53OjI1PO5zud32DkMALso9Eo/FkMoUnmYGq9HjfwB7ay7Q2Gn9xncdDuxhQ1XbX9zJKH0P3DFi3giq8ndZvwYxKEEQ0GrdYbLLDY8GOSKPVw7SBEzmj2lUmkw0GQxarHTJSOZxuaBxqTITDkWAw5PF4jefmVQ7v+YvXL16+QTGDyImu0Uyk1/Qa/4s6vFarO5zuufmlP337Z/6GAIrc4H53lUrl8vIKIIMkSRQlk0ikgFVETUHxG/SkMA7VZnE3IDxADP0QHFkLhWKnExLOecaQokHweLxGo0l+pFxc4oyMTs7NL+2JDlwuD+xJPOz2RwxYjGVMXE/GgseHkx0iVzoRHIdwLjLGEJepke8I+qpcLofDkaVlrkKpApjbFuy5PV50DRTirlSqk1Msl8szNj4N38J8FYtFPNKIbrLhrY/fy1MAtDEAq5W3+tIB697RCp1gbWWiYrEI3IfV5tjd2wf5y+Pxgsx1cqqGkmoqtdbnC+RyeUhSrNWdmczWQOASD8UCX0pIPntyquZw+VLZ0cWFD2pbgCQPjwDmoXg8Cc5yDG8j2PZerx/y1UJtZKlMHonEAFnqzbomuD8xrlCAkbm6CitPVGazNRqNA29VLBahCDPO4ZOYP0Hb4FIANUYWCr8/6PX6HU63xWoH7zCv1+/2eI3n5mPFyY5QDLFy4GsKGjcUhobzFD8RwGq7mPGhvtXpi1rrshHgczTUcDFkwSUIwu5wgaEZKad8voDPFwDFCEVRwKdvC3ZVai1N0/WWwl94T+48SriA3FYSvPPG/0i6f8DqsTUSC3/rlE8nEonp9AaT2ep0upUnqj3RAUrLWalUwWSj0xvODOcarV6nN6C4GaDWUE+aphXK0xcv3wwMjqytbxqNJqjXAEmEoUYDmNi6d75eb/j9QZVaKxJLoLL58soaWNwymSxCARAK6vVGNpsDB1HwqNbqzvgbgh2h+OhYqVJrlSeq5ZW1Pz/54fd/+GZPdAAQ2TbFIENLlcvlPR6v8kS1IxQbjKZIJKrW6MAVEJwSxftScGEXiSUcLp81twjFO+0OVxenBOTK230QvkZqC1h3awc/TnDvdsb2xr1tyaZWCJY9VIrOZnMQlpBIpCKRKEmSBqOpr38oEolC+ct3fe8PJIfo1otLHJPZCuVOqevxQ4ywZ9RJ9O+tHrYXWP/4kbwtfU7AamAJBmotSY1pmgYnTKvN4XC6odA2uD5RFFUoFA1Gk8Vqj8USPP6WSq21O1yQ3gxNVWvs29Iy99vvnnC4/LHx6Xd97xfYK6CN4q5t8PjbsLcHBkd+/4dvZIfH3ftfqVRhSV1c+LYFezOzC+/63j999vLFyzcL7JVTlcbvDyJx0uXyrPO2hobHnz578eLlG0iVEw5HpDI5a27x/dDYjlBsMlv5G4K+/qEn3z8ViSUIL+r1BmTIae0D6MiWlrnf//D8zdt+9uKqVCaHcFmXy+N0usH53uPxopDAWq1usdh8vkAX9Xyn2IMfB90LVOFSJArYxK2KiHAtGNo7gFmgfgJjIig34Ih1uy9evnobCFyCNmDw/ahao0Onl/JEdW6ygPBIX89QBv3BJ466XsH3Vk/dFtw/L1rRdwOsj0crGkucAl5LeBA5RVEAYXPzSxBcAumiwuEI7NtisXh5eaXTG0DnPTE5a7HYgLeiKCoSiaZS6bahT+MTM3/85luymXCDoqhKszoWTdOZTFanNywtc4eGx4HfTqcz3X2UUO4t5YmKx98S7IgkUjmHy5+cYnG4fKlMfqw4OVacbAv2NFq9233B4fK//e77oeFx4a54W7An2BG5XB6apqGMs98fPFacLC5xlpa5/A2BeF+q1uhsNsfVVbjVsxSSz4F5e3xi5lSluXH8CYLIZnORSCyZ7OYciDiCHyVgfQwhuGGovVrNI4yftI4k2Yw9Bja81qzVBMz40PA4xEtVKlX24qrX64dgCZh0s9n6/MVrKJjKAKxWrrwt7tw4s51+dbfW7pE+G2BRTesv+ApBWl78ArPZarU54K/H441EongZcbvDBSEFZrNVvC9F5g+IZQUbM95gpVKNxRKTU6yV1XW4O/KiQgJgJpM1Gk2CHdECe0WwI9LqzmAF4C42OEHkdjyeNBpNOr3BaDQBaEYisZNTNcRqLS1zxfvSdDoDWlXoZDAY2hMdcLh8/obg8vIKWru8vIKEhSq1dk90sMrhjY1P9/UPseYWBTuizS0hVKazWGxQgxP8EkViyalK4/Z4WwsR4lSvN7S6M/biqnBXDPH3jCdibMWfIGB1337Ude8HBlTdTYKGM5vhiwuxijz+9o5QTNN0pVJdW99EqTKq1Zrd7rTZHE+fvYTc87ho391ZoXXn3haVPiNOIfr8gAX+RK2AtS3YpWl6/0BmMlvD4QhuFysUisB3gKsxKtAUjycZhb9A3V4oFGOxBBQonZxiPX328v3Q2CqHtyMUyw6PIRCfpmmoDq/W6CCh+8DgyNz80tz8ks8XaNX4NBoNlMIBuoQyBdLXVaHIWoQeMB5P6vSGkdHJ//zP365yeKA4g1w0u3v7e6ID/oaAvyHQ6s7wQlulUkm4K2bNLS6wV4aGx1+/6R+fmAFvdYvVHo3GW5mmRqORTmfAXcPl8ni9fr3eIJXJLRYb7v1ANgvE1rFUfz8pwLpxZ7ZCFYpS+khwx88JJPjr9Yax8Wmapuv1hmBHhLxeGo0GqEpfv+mDQEK0MimK6u6MQrbzq2q7l3sBtbs97MdTr4DFmLyPByy6mY6jWc77gwQHmyccjkik8mq1pj8z+nyBTCaLJ1aHa9wer+zwWCKVo70H7aBOAmChWPx0OgPqBsj6em6yOJ1uDpf/4uWbH54+93r9uNhVLpddLs+Ll29evHzDXly1digbEwqFVWotvFB+/laCEByapu0OF4+/PTU9NzY+zV3bgDrDS8tc9uLqKoe3LdjT6s7cHu+pSrMt2DMaTXjeS3De8Xi8Wt2Z0Wjyev04jEKOZoi2T6XSiUQK6jBC0JLPF4BSdFDeEVUhhLlDBzuuNm4ryPyI6UbAwpVWnTIj3vmm8C+aUKfT3dc/BO/3D2SBwCWEoxIEweHy7Xbnu75Bl8uDJ54EDqBTN9Aj4EaAtvTFQhXQ5wQsGiu2XGvWnqlWa+CsAPWQQ6EwoBXcAnzk4LdnhvOjYyUDaGgshzKjP5VKFXRb6BMIELu6Cv/w9LlUJhfsiMT7UuWJSn9mPJAccrj8cpMgwwY6vvBzzGKxDY9M/P4P3/z2d39AHphAhUIR2rc7XKcqjUgsmV9YHp+YUam15HUPHRhVFISEeg5ri8K0e+hXIGM6nW67wwUxzy6XB/LEW6x2EJYdTrffH4zFEm3zhVax6kF4InDi80WKfQnUdn8iwMLTIuJuSrcdK+p6Bn10F3gTCoXf9b2HKnAK5enJqRrUtY1GY3Rsymy2DgwOQ8Q13mCXblCYp0JbzOqRsfrsS+IzAxZqvIaV59oTHSiUKsh9EYslcG1LtVrL5fIwr1LZEV58FG8NutSLWoEgiEKhqFCqHE63cFc8v7Cs1uiSyZRCqRoZndw/kO0fyKLROCQbIVtcqxKJ1IHkcGp6jsPlH8oVJ6dqCN93Ot3ifenkFGtmdmF5ZW2Wxe7rH3rX9/5QrgDht1PCg0bjQ1RHL3E25XI5Hk9eXl6Bwj4UCsdiiVQqHY3Gw+HI1VUYGC5wEANCj1DvUB8Mt4LfOHo/HaKaxdDwJK6AWa0+or0Q4ndafwhz0T8wrDxR0TTt8XghfS5N09Vqra9/SKPVDwwOgy4FLZIeAattXrPe0eqzY9Y9pEjuToyHpJqsKZpyiCGAgyuXy29tC5UnKqvNEY8nwdYLmdVAlQ4Fr66uwkvLXJvNQZLk3ZKcoPMNvMnBrtxqYQHOxWy2QsCNVHYkEku2BbubW8LdvX35kVKj1V9c+BgBxvhdGp2zGgDwJRKpUCgMvNix4kR5ojoznEOSP6TAAtwB39dkMgWhy5DnfmmZy+NvSaTyYDAE49xqHyAxw9/dXHJ+mnTjvr3zlqYwpRjupQXfghCwtMzd2hZSFHUgOXz56u3VVRiuyWSykUhsaZkLeXHhdrCS2x5y1HVzytd+Gj0C1iNgPVJ7egSsL5AeHLDoFvMijB3yx6VpmiCIdDpzceHbP5DNLyzDhxcXPqfTnc3m8A2vPzOGwxGd3iASS+5Wx4WxsNpywm1/1epog6s8Wwkc3CORKKSyAccr8E5YW99cW9/c3BKKxBL5kRKSdsmPlMMjE8MjE6y5Re7axoHk0Ol0o2htaAoMBbFYIhqNQxWmbcHu/MLyzOzCoVwRicQggIPRc/J64oEeN9Uj0R+BWTc22wWwQOGwwF5ZW98kCILH34Ii5JBaL5fLp1Lp90NjkUgUN/WCxNoJsEjMRPhVz/6nAyw0Q63nPFjTLRYbh8s3m631egPcLNPpDI5W5XIZCvmJxJKLCx8+Nz1qEFBPOi0sUCGBv0I2m/N6/V6vv5kbL5pIpPBa4d1nnSCISqUKy6vRDKiuN2vw4sHPdFMbRdN0pVJJJFK5XB4ua0b8fSD0byaTjUbjwHZB+WiIf4QATBpbpvib2+6rR3ogwKKvezMgzIKvALBYc4uLS5xKpcpd29DpDZBIHiSSSCQ6Mjrp9fqRLyHduaApWvNIx/9VT/0nAiwSc2PBFY0wdiDFgNM2TdORSPTN2348VJ2m/3/23rSrkSRNF/w5/Q/6y9wz0/OpP97Tp+9Mn749c2/PPX2rurpvVld3dVV1VWVW7ktkxr5HQAREQAABAQKxCyRWgRAIhHYhISGE9n11Sb7Nhydlabi7hCCICIjQe/LkIVzu5uZmrz322ruKHMcFgyHjpkmrW1KPT9E/8TyPSK4TYUugRCrFOUPCPDgERCJR+ENNz8zpFpbX1jc2t7Z3LTav14fEniSRCG1OFurBEE14goCm5DqprQLfMWRZQvIZyc0syxaLxXQ6k0ymMpksKsuz9cqa8gOg5O1tzGqR3hxgCUpCFn7CjtjV3dvV3ZvPF0ZU49FoPBKJghmSydTh4dGTp89tNkckEqMbVLRX0oDVhPMvC709wGLr7gvyMYVyalajtdkcDMMYNjZ7X7wMBIKSdnbMlrX1jemZOadrjz/uFtA6YAmUhCW/oVb7CQgSiRS0bJIOI8ELYIJUlCFtEi48rdlI3lU6dEN+A+F19I3wq1yMbTQObcw6kd4mYJETAyQsAFY8nlzVG5yuPURE1GosAip6egc2jFuS8tSKOyXdq8suXonnVfn5xNu4n+oSV+TH7HK57HC4VKMToii63J7hEbVp2xyJxCTqGN3Ckm5hWbewJIpiLpcnvxJhuPUON2Is7qfScscyYcFKAAdU4iUg8VqSaAokOiPy9kYbnbwzLMsSNDzxo+ibT9xLz7DAPkx6C4BFYxZ+gtL92fO+5z39kUgUhXYAWBzHTU5pCoXi8Iga6f3od8nP/oofcr5D9JbptQCr9SEAYAEIFJHl5eAI0uwbNjanpjW7FhvSA3FUOI5uYXlwSIXEAxCpyPpsfgRr1G3huD7yRFzgKXOb3JlFTooa/UaDptj/1i/yp0wkcoY19gHSGaCqxcEk7KcEWIwoiqjlVSqVkHyN5BedmJwNhcJr6xuwIUpW03s/p28JsPifSuAqA9Z3V65GIlFRFLW6pQ3jltVqh1McHaywvKLv6Owmj0AIYk9f35FGK5ZyX5ab/BSxRr4xKoIXr0T0cJHWWlcuKBr7JH1rcTTOsMY+QGoRns42mIIMsPAgVLqwEoqiODmlmZmdx+pAlTnUiBt4OSxfTcJJWtrLTmcHrFNNj1B3FVHM+hKNxh89fgofq1X9usvtgeY7nc6Qc5nVap+YnMWxEUQUTG8OsJo3Ij8DNoGqJoDVRNkkoRPvFBqo85sMQhuwmtDbBCzCfojN6nzybGZ2XhCEl4MjpD4YzhlO114ul4crlvxdbcBSoLNNDw6GOHlBdBIEoVwuz2sXjZumSqUaicQ8Xh/QKhAIImWKIAgMU1nVG170DZJCNfTp7LTTQwMWvb+deCRs1BoNW03Qipcd1s4whs3vFI47MTRvpw1YJ9KbAywJ29AaiWKxyLLs3XuPUJNiYnLW4XBxHFcoFLPZnNlsQf5F1eiEcdOER2g54FRb4KWjtwdYkgcLhR9zrpt3rTirY8Qx1sMj6oODQ6EeAFUsFgdeDvcPvMpkssViUagHpgunF4Bfn9VabPZs7TRpvMU7FZX9J/b2vWTu16cTueXMXCQcd+ilH0GZqHv3H4+pp6xW+8HBIamSCy+WcDjCMMyGcQtuQDzP0+6BfF2b2TrPXCIGOAtgvT6vC4KAaguiKK7qDa+Gx1gqhMXhcG0Yt2KxBBwvEbjz5OlzFEzF2Q3/byS5nKrzF3n1ojOn0kzJlVyKbV7M771o1CK3nGE8BQqwJPdjady5+3B0bNLl9gQCQZRrhZIEZVALheLBwSE8S1GbkjTC8/ypMt5cLk54Z4AFuVcURc2cbm5+Acnd8evE5CxSdCaTKSQhqFZrDx52opwkW0/MSKq8nKoDb4L5zkyN3oIrBI5bP/YKMi3+O//GS01n4JYWx1M4nu6dXBTrR8Jbt+9Pz8wdHh45ne5V/brT6U6nM9Dzwm+xUqm+HBzxen0k4RIe5+sFnFuc1svFDOcDWKf9SEEQkGxPFMXBIZXFaofXuCiKMNlC74gyMMiB9fDRk1KphMxz5L8z5E47FdtJrHKn+sYWeyLXc0lU+OzxNCBNutGowRPB63y/632iU3HLqYaUpyLV6IuiKCIa/+q1m1umnVQqvbi0OjM7v2uxFYs/1uIk1TPn5hempjUkbSRACuePJsn8WvnGswzWW6F3A1jijzY+RhTFru5eRB4gpyLqDMKFNxAIzmq0oig6XXtPnj4XRRHpQwF25XL5DKa9Jp2XX6dTBp8jZpH2aYSC4p8k+ZZk+2ZlMZiK1AitmiDXuXzR+0pNhro5ndhyE8CqVKqhUPjGzbvBYKhUKr0aHhtRqU2mHURuIUAH95t3rZ1PnpFawqQsZuuAdeb+vyt6Z4AF4SgWSzx5+jyXyyeTKZQ8Mm2bg8EQ9Fl2h8tk2qnV2B2z5dnzPkEQUGUHATEArBYd3Bv1XPEGsrYlae3OayLJ2yWAJUcrGrNaASzh9Jh1Ll/0vlLzoW5CrbTMKYVwwfdwcWl1fGK6Wq2lUmkk0davGbLZHEknj5v9/oBWt7SqN8AhC2sBLbc4s2fu/7uidwZYGFzTtvl5Tz+EplKpFAgEXW5PJBJFg6ZtM4ohbxi3el+8rGcr/jE1bYtpOZv3XH4DvbAltcvPayLJ21uRsCSFIeTdkHxRG7DOkVrBpjMvB55KkQyPH1EUy+VyPl/o6R1ANt1QKLyyutb97IVuYTkSicIUyNdrmqRS6VAo/LSrJxyOpNOZM8zm6/T/ndA7AywM+vCIempagzQpxWLx4ODQ6XRDpkX1eaRDWF7Rd3X3opQDFIosyxLAav3tJ3ZbOA4idKbzNwdYvCwItglgNeqDvM02YL0+nQKiTr8cBCoaGYHuoihWKtUt0868dhG5rhKJ1LrB+LynXzOn29/3E9mK53mk9EgmU0vL+pnZeZfbc44feIam3g69bk73VtTS5CncwHEcNgq32/Po8VPYOBiGCYcjU9OadDqDbFCFQtHt9qytbxQKxaOjcF//EAKeEUFdKpUQh8zLvD25uks9KR7RPNNei199vszapotPrzmtQuNQCiAUNmkcGtD+qt6gHp9C4RWyapyuvVmN1mK1I+oe/Ix2dswWrW4JVYc1c7qZ2fn9fT9U8lhu2PiRTZdeKaRv9DJpFGbP10tVS+qVSAT/c9zRm1AbsFr96jZgfWjUBizQpQQsQieuVeEkR0cUZ65Wa70vXqZSaUi5+jXD9Rt36JrstRq7t+ddNxjxz6ddPbqFpXQ6c3h4BL0VJk9xiEUqdoc9nn/2HD+2DVjvPZ3vtAqCAKbFP1mWJWn7dy02lPj2+wOzGu3klAY3I/ltPl9ATQO6G4lEqlZjtbolp9ONNiuVqnp8SqtbikSiuVy+UCiSDZt4ZQv1OgM03DQHHaKyoCstSQxB/Gmct1+Hzic0hxANxopCDV8v/eDx7C8sroiiyDBMMBia1Wgfd3QhSAp3chxnd7jg1iCK4ujY5LPnfXaHiyQt4+qJ4WHrVcy09ZrUBqwPnFqfVvpO2uareAKgjYP5fMG4aerq7v32ux+Mm6ZIJDo1rXk5OLJl2tnf9+fzBWQlEerSABg+Fku43J5EImWzOxOJFFADS8PucPX1Dw28HNbqlvb3/eS9LMvS5dMVSa4nJYtaolpVRKuLC1hyIoDF1su3KcIHZKJajV3Vr6M2ZCyWMGxsogKgze5EVW6o0m12p3p8CvXXMpms2+3Rrxl0C0tIRirUo6lzuTxJ7dB8yEgnFdXP50XnNaRteufU4sxKmIplkauSkWTuxxEM4gnDMKR45fUbd2Y12kQiJdZ9qlF8NxAIZrO5QqFIKiEh220wGLLZHJtb2/v7/kKh6PHsa+Z06vGpMfXU4tLq4eFRtVpLJFJ2h2ttfWNWo9XM6ZZX9FarPRKJNqrhRHpIu4aR9UJ73tCnFvkKOodBb0pvJEWyXLYUqExj8XjS6XTvWmzwdDdumh487JyYnD0</t>
+        </is>
+      </c>
       <c r="I72" s="3" t="n">
         <v>1</v>
       </c>
@@ -6100,7 +6412,11 @@
           <t>We can use heat for all the following except _______.</t>
         </is>
       </c>
-      <c r="H73" s="3" t="inlineStr"/>
+      <c r="H73" s="3" t="inlineStr">
+        <is>
+          <t>We can use heat for all the following except_______.</t>
+        </is>
+      </c>
       <c r="I73" s="3" t="n">
         <v>1</v>
       </c>
@@ -6177,7 +6493,11 @@
           <t>Which one of the following is an oil crop?</t>
         </is>
       </c>
-      <c r="H74" s="3" t="inlineStr"/>
+      <c r="H74" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is an oil crop?</t>
+        </is>
+      </c>
       <c r="I74" s="3" t="n">
         <v>1</v>
       </c>
@@ -6254,7 +6574,11 @@
           <t>Which one of the following tools should not be shared?</t>
         </is>
       </c>
-      <c r="H75" s="3" t="inlineStr"/>
+      <c r="H75" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following tools should notbe shared?</t>
+        </is>
+      </c>
       <c r="I75" s="3" t="n">
         <v>1</v>
       </c>
@@ -6331,7 +6655,11 @@
           <t>Which one of the following is a natural source of light?</t>
         </is>
       </c>
-      <c r="H76" s="3" t="inlineStr"/>
+      <c r="H76" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is a natural source of light?</t>
+        </is>
+      </c>
       <c r="I76" s="3" t="n">
         <v>1</v>
       </c>
@@ -6408,7 +6736,11 @@
           <t>Which one of the following tools is not correctly matched with its use?</t>
         </is>
       </c>
-      <c r="H77" s="3" t="inlineStr"/>
+      <c r="H77" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following tools is not correctly matched with its use?</t>
+        </is>
+      </c>
       <c r="I77" s="3" t="n">
         <v>1</v>
       </c>
@@ -6485,7 +6817,11 @@
           <t>Bile produced by liver is added to food in the _______.</t>
         </is>
       </c>
-      <c r="H78" s="3" t="inlineStr"/>
+      <c r="H78" s="3" t="inlineStr">
+        <is>
+          <t>Bile produced by liver is added to food in the _______.</t>
+        </is>
+      </c>
       <c r="I78" s="3" t="n">
         <v>1</v>
       </c>
@@ -6562,7 +6898,11 @@
           <t>Which one of the following can float in water?</t>
         </is>
       </c>
-      <c r="H79" s="3" t="inlineStr"/>
+      <c r="H79" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following can float in water?</t>
+        </is>
+      </c>
       <c r="I79" s="3" t="n">
         <v>1</v>
       </c>
@@ -6639,7 +6979,11 @@
           <t>Which one of the following foods is not a source of energy to the body?</t>
         </is>
       </c>
-      <c r="H80" s="3" t="inlineStr"/>
+      <c r="H80" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following foods is not a source of energy to the body?</t>
+        </is>
+      </c>
       <c r="I80" s="3" t="n">
         <v>1</v>
       </c>
@@ -6716,7 +7060,11 @@
           <t>Which one of the following is not an industrial use of water?</t>
         </is>
       </c>
-      <c r="H81" s="3" t="inlineStr"/>
+      <c r="H81" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not an industrial use of water?</t>
+        </is>
+      </c>
       <c r="I81" s="3" t="n">
         <v>1</v>
       </c>
@@ -6793,7 +7141,11 @@
           <t>Which one of the following foods is not digested right from the mouth?</t>
         </is>
       </c>
-      <c r="H82" s="3" t="inlineStr"/>
+      <c r="H82" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following foods is not digested right from the mouth?</t>
+        </is>
+      </c>
       <c r="I82" s="3" t="n">
         <v>1</v>
       </c>
@@ -6870,7 +7222,11 @@
           <t>Which one of the following happens at the same time when the diaphragm forms a dome shape?</t>
         </is>
       </c>
-      <c r="H83" s="3" t="inlineStr"/>
+      <c r="H83" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following happens at the same time when the diaphragm forms a dome shape?</t>
+        </is>
+      </c>
       <c r="I83" s="3" t="n">
         <v>1</v>
       </c>
@@ -6947,7 +7303,11 @@
           <t>A lot of water for a town can be stored in a _______.</t>
         </is>
       </c>
-      <c r="H84" s="3" t="inlineStr"/>
+      <c r="H84" s="3" t="inlineStr">
+        <is>
+          <t>A lot of water for a town can be stored in a _______.</t>
+        </is>
+      </c>
       <c r="I84" s="3" t="n">
         <v>1</v>
       </c>
@@ -7024,7 +7384,11 @@
           <t>Which one of the following can be learnt about soil from the set up below?</t>
         </is>
       </c>
-      <c r="H85" s="3" t="inlineStr"/>
+      <c r="H85" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following can be learnt about soil from the set up below?</t>
+        </is>
+      </c>
       <c r="I85" s="3" t="n">
         <v>1</v>
       </c>
@@ -7101,7 +7465,11 @@
           <t>Which one of the following is not a fibre crop?</t>
         </is>
       </c>
-      <c r="H86" s="3" t="inlineStr"/>
+      <c r="H86" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is not a fibre crop?</t>
+        </is>
+      </c>
       <c r="I86" s="3" t="n">
         <v>1</v>
       </c>
@@ -7178,7 +7546,11 @@
           <t>The second part of the alimentary canal is _______.</t>
         </is>
       </c>
-      <c r="H87" s="3" t="inlineStr"/>
+      <c r="H87" s="3" t="inlineStr">
+        <is>
+          <t>The second part of the alimentary canal is _______.</t>
+        </is>
+      </c>
       <c r="I87" s="3" t="n">
         <v>1</v>
       </c>
@@ -7255,7 +7627,11 @@
           <t>The first stage of HIV and AIDS</t>
         </is>
       </c>
-      <c r="H88" s="3" t="inlineStr"/>
+      <c r="H88" s="3" t="inlineStr">
+        <is>
+          <t>The first stage of HIV and AIDS infection is ____.</t>
+        </is>
+      </c>
       <c r="I88" s="3" t="n">
         <v>1</v>
       </c>
@@ -7332,7 +7708,11 @@
           <t>The following diagram represents a type of tool used in the farm.</t>
         </is>
       </c>
-      <c r="H89" s="3" t="inlineStr"/>
+      <c r="H89" s="3" t="inlineStr">
+        <is>
+          <t>The following diagram represents a type of tool used in the farm.The following are ways of maintaining the tool above. Which one is not?</t>
+        </is>
+      </c>
       <c r="I89" s="3" t="n">
         <v>1</v>
       </c>
@@ -7409,7 +7789,11 @@
           <t>At which part of the alimentary canal does egestion occur?</t>
         </is>
       </c>
-      <c r="H90" s="3" t="inlineStr"/>
+      <c r="H90" s="3" t="inlineStr">
+        <is>
+          <t>At which part of the alimentary canal does egestion occur?</t>
+        </is>
+      </c>
       <c r="I90" s="3" t="n">
         <v>1</v>
       </c>
@@ -7486,7 +7870,11 @@
           <t>Which one of the following is a weed that grows along the ground?</t>
         </is>
       </c>
-      <c r="H91" s="3" t="inlineStr"/>
+      <c r="H91" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is a weed that grows along the ground?</t>
+        </is>
+      </c>
       <c r="I91" s="3" t="n">
         <v>1</v>
       </c>
@@ -7563,7 +7951,11 @@
           <t>Water can be used for fun when _______.</t>
         </is>
       </c>
-      <c r="H92" s="3" t="inlineStr"/>
+      <c r="H92" s="3" t="inlineStr">
+        <is>
+          <t>Water can be used for fun when _______.</t>
+        </is>
+      </c>
       <c r="I92" s="3" t="n">
         <v>1</v>
       </c>
@@ -7640,7 +8032,11 @@
           <t>HIV and AIDS cannot be transmitted</t>
         </is>
       </c>
-      <c r="H93" s="3" t="inlineStr"/>
+      <c r="H93" s="3" t="inlineStr">
+        <is>
+          <t>HIV and AIDS cannot be transmitted by ____.</t>
+        </is>
+      </c>
       <c r="I93" s="3" t="n">
         <v>1</v>
       </c>
@@ -7717,7 +8113,11 @@
           <t>Which one of the following animals is wrongly matched with its product?</t>
         </is>
       </c>
-      <c r="H94" s="3" t="inlineStr"/>
+      <c r="H94" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following animals is wrongly matched with its product?</t>
+        </is>
+      </c>
       <c r="I94" s="3" t="n">
         <v>1</v>
       </c>
@@ -7794,7 +8194,11 @@
           <t>The stem of a plant can do all the following except</t>
         </is>
       </c>
-      <c r="H95" s="3" t="inlineStr"/>
+      <c r="H95" s="3" t="inlineStr">
+        <is>
+          <t>The stem of a plant can do all the following except ____.</t>
+        </is>
+      </c>
       <c r="I95" s="3" t="n">
         <v>1</v>
       </c>
@@ -7871,7 +8275,11 @@
           <t>Gastric juice is produced by _______.</t>
         </is>
       </c>
-      <c r="H96" s="3" t="inlineStr"/>
+      <c r="H96" s="3" t="inlineStr">
+        <is>
+          <t>Gastric juice is produced by _______.</t>
+        </is>
+      </c>
       <c r="I96" s="3" t="n">
         <v>1</v>
       </c>
@@ -7948,7 +8356,11 @@
           <t>In which of the following parts is food absorbed?</t>
         </is>
       </c>
-      <c r="H97" s="3" t="inlineStr"/>
+      <c r="H97" s="3" t="inlineStr">
+        <is>
+          <t>In which of the following parts is food absorbed?</t>
+        </is>
+      </c>
       <c r="I97" s="3" t="n">
         <v>1</v>
       </c>
@@ -8025,7 +8437,11 @@
           <t>In which one of the following parts of the digestive system does digestion end</t>
         </is>
       </c>
-      <c r="H98" s="3" t="inlineStr"/>
+      <c r="H98" s="3" t="inlineStr">
+        <is>
+          <t>In which one of the following parts of the digestive system does digestion end?</t>
+        </is>
+      </c>
       <c r="I98" s="3" t="n">
         <v>1</v>
       </c>
@@ -8102,7 +8518,11 @@
           <t>Which one of the following foods is a source of proteins?</t>
         </is>
       </c>
-      <c r="H99" s="3" t="inlineStr"/>
+      <c r="H99" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following foods is a source of proteins?</t>
+        </is>
+      </c>
       <c r="I99" s="3" t="n">
         <v>1</v>
       </c>
@@ -8179,7 +8599,11 @@
           <t>Which one of the following is both oil and food crop</t>
         </is>
       </c>
-      <c r="H100" s="3" t="inlineStr"/>
+      <c r="H100" s="3" t="inlineStr">
+        <is>
+          <t>Which one of the following is both oil and food crop?</t>
+        </is>
+      </c>
       <c r="I100" s="3" t="n">
         <v>1</v>
       </c>
@@ -8256,7 +8680,11 @@
           <t>HIV virus cannot be found in _______.</t>
         </is>
       </c>
-      <c r="H101" s="3" t="inlineStr"/>
+      <c r="H101" s="3" t="inlineStr">
+        <is>
+          <t>HIV virus cannot be found in _______.</t>
+        </is>
+      </c>
       <c r="I101" s="3" t="n">
         <v>1</v>
       </c>

</xml_diff>